<commit_message>
added a second echelon. Still functions as expected
</commit_message>
<xml_diff>
--- a/DEAS_Equipment.xlsx
+++ b/DEAS_Equipment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronnie\Desktop\DEAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B953D90A-A260-4964-9416-BC34D313E643}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E57263-A3BF-4FD0-B0EB-4E9ED32DB4E3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Event Room Arcs'!$A$1:$J$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Movement Arcs'!$A$1:$J$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Movement Arcs'!$A$1:$J$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Room Inventories'!$A$1:$C$1771</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Storage Room Arcs'!$A$1:$J$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Utility Arcs'!$A$1:$J$4</definedName>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="30">
   <si>
     <t>Storage Room</t>
   </si>
@@ -1844,11 +1844,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView zoomScale="89" zoomScaleNormal="54" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2018,7 +2018,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2027,7 +2027,7 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -2059,7 +2059,7 @@
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -2077,6 +2077,134 @@
         <v>72</v>
       </c>
       <c r="J7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>72</v>
+      </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>72</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>72</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>72</v>
+      </c>
+      <c r="J11">
         <v>0</v>
       </c>
     </row>
@@ -2088,11 +2216,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2164,6 +2292,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>72</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J3" xr:uid="{DB8A11DE-3284-4D20-A701-318DCC0FB799}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2172,11 +2332,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2245,6 +2405,38 @@
         <v>20</v>
       </c>
       <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>0</v>
       </c>
     </row>
@@ -2260,7 +2452,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2369,7 +2561,7 @@
         <v>29</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
@@ -2378,7 +2570,7 @@
         <v>29</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
added a second commodity. Still functions as expected
</commit_message>
<xml_diff>
--- a/DEAS_Equipment.xlsx
+++ b/DEAS_Equipment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronnie\Desktop\DEAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E57263-A3BF-4FD0-B0EB-4E9ED32DB4E3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31EF4D7-4F78-488F-9B24-4B2229D277E5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Room Inventories" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="31">
   <si>
     <t>Storage Room</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>t</t>
+  </si>
+  <si>
+    <t>TABLES</t>
   </si>
 </sst>
 </file>
@@ -647,11 +650,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -683,6 +686,17 @@
         <v>72</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -694,7 +708,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -720,13 +734,23 @@
         <v>25</v>
       </c>
       <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="C2">
+    </row>
+    <row r="3" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
     </row>
@@ -1844,11 +1868,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView zoomScale="89" zoomScaleNormal="54" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2208,6 +2232,326 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>10</v>
+      </c>
+      <c r="J13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>10</v>
+      </c>
+      <c r="J14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>10</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>10</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>10</v>
+      </c>
+      <c r="J17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>10</v>
+      </c>
+      <c r="J18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>10</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>10</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>10</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J7" xr:uid="{96EB14DA-D016-4997-9091-5CA43F8416A6}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2216,11 +2560,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2324,6 +2668,70 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J3" xr:uid="{DB8A11DE-3284-4D20-A701-318DCC0FB799}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2332,11 +2740,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2440,6 +2848,70 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5">
+        <v>9</v>
+      </c>
+      <c r="I5">
+        <v>9</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J3" xr:uid="{62F394A8-9F05-4E55-93AD-A5A4A265C3A8}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2448,11 +2920,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2588,6 +3060,102 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J4" xr:uid="{BCC15CB7-F490-4A4D-8BC1-B0D4AB66EEE8}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
doubled the rooms considered. Still functions as expected
</commit_message>
<xml_diff>
--- a/DEAS_Equipment.xlsx
+++ b/DEAS_Equipment.xlsx
@@ -8,27 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronnie\Desktop\DEAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31EF4D7-4F78-488F-9B24-4B2229D277E5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819B554B-5646-489B-9381-AE775F5D3B3A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Room Inventories" sheetId="1" r:id="rId1"/>
-    <sheet name="Commodities" sheetId="2" r:id="rId2"/>
-    <sheet name="Storage Rooms" sheetId="3" r:id="rId3"/>
-    <sheet name="Cost Data" sheetId="4" r:id="rId4"/>
-    <sheet name="Event Requirements" sheetId="6" r:id="rId5"/>
-    <sheet name="Movement Arcs" sheetId="7" r:id="rId6"/>
-    <sheet name="Storage Room Arcs" sheetId="8" r:id="rId7"/>
-    <sheet name="Event Room Arcs" sheetId="9" r:id="rId8"/>
-    <sheet name="Utility Arcs" sheetId="10" r:id="rId9"/>
+    <sheet name="Deployed Units" sheetId="11" r:id="rId2"/>
+    <sheet name="Commodities" sheetId="2" r:id="rId3"/>
+    <sheet name="Storage Rooms" sheetId="3" r:id="rId4"/>
+    <sheet name="Cost Data" sheetId="4" r:id="rId5"/>
+    <sheet name="Event Requirements" sheetId="6" r:id="rId6"/>
+    <sheet name="Movement Arcs" sheetId="7" r:id="rId7"/>
+    <sheet name="Storage Room Arcs" sheetId="8" r:id="rId8"/>
+    <sheet name="Event Room Arcs" sheetId="9" r:id="rId9"/>
+    <sheet name="Utility Arcs" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Event Room Arcs'!$A$1:$J$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Movement Arcs'!$A$1:$J$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Event Room Arcs'!$A$1:$J$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Movement Arcs'!$A$1:$J$73</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Room Inventories'!$A$1:$C$1771</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Storage Room Arcs'!$A$1:$J$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Utility Arcs'!$A$1:$J$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Storage Room Arcs'!$A$1:$J$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Utility Arcs'!$A$1:$J$4</definedName>
     <definedName name="Commodities">Commodities!$A$2:$A$3</definedName>
     <definedName name="Rooms">'Cost Data'!#REF!</definedName>
     <definedName name="StorageRooms">'Storage Rooms'!$A$2:$A$3</definedName>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="34">
   <si>
     <t>Storage Room</t>
   </si>
@@ -140,6 +141,15 @@
   <si>
     <t>TABLES</t>
   </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>Useful?</t>
+  </si>
 </sst>
 </file>
 
@@ -176,7 +186,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -299,11 +309,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -312,9 +352,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -324,16 +361,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -650,11 +697,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -683,7 +730,7 @@
         <v>25</v>
       </c>
       <c r="C2">
-        <v>72</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -694,7 +741,29 @@
         <v>30</v>
       </c>
       <c r="C3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -702,13 +771,403 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="7" max="7" width="12.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>12</v>
+      </c>
+      <c r="I2">
+        <v>12</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6">
+        <v>50</v>
+      </c>
+      <c r="I6">
+        <v>50</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10">
+        <v>72</v>
+      </c>
+      <c r="I10">
+        <v>72</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:J4" xr:uid="{BCC15CB7-F490-4A4D-8BC1-B0D4AB66EEE8}"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3400B00F-A93C-4A24-A597-B4693608C43F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -792,13 +1251,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -825,12 +1284,12 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>80</v>
-      </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -994,15 +1453,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1010,36 +1469,88 @@
     <col min="1" max="1" width="10.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="C1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7">
+      <c r="B2" s="16">
+        <v>0</v>
+      </c>
+      <c r="C2" s="16">
+        <v>5</v>
+      </c>
+      <c r="D2" s="16">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="8">
+      <c r="E2" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="16">
+        <v>5</v>
+      </c>
+      <c r="C3" s="16">
+        <v>0</v>
+      </c>
+      <c r="D3" s="16">
+        <v>8</v>
+      </c>
+      <c r="E3" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16">
         <v>7</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C4" s="16">
+        <v>8</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="7">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7">
+        <v>6</v>
+      </c>
+      <c r="D5" s="7">
+        <v>2</v>
+      </c>
+      <c r="E5" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1048,7 +1559,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H129"/>
   <sheetViews>
@@ -1068,28 +1579,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="11" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1866,13 +2377,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView zoomScale="89" zoomScaleNormal="54" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1881,34 +2392,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1955,7 +2466,7 @@
         <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1973,12 +2484,12 @@
         <v>72</v>
       </c>
       <c r="J3">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1987,7 +2498,7 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2010,7 +2521,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2019,7 +2530,7 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2037,7 +2548,7 @@
         <v>72</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -2045,7 +2556,7 @@
         <v>27</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -2054,19 +2565,19 @@
         <v>27</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="s">
         <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -2077,60 +2588,60 @@
         <v>27</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="s">
         <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="J7">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="s">
         <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="J8">
         <v>7</v>
@@ -2138,51 +2649,51 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="s">
         <v>23</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F10" t="s">
         <v>23</v>
@@ -2197,24 +2708,24 @@
         <v>72</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11" t="s">
         <v>23</v>
@@ -2234,7 +2745,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -2243,7 +2754,7 @@
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -2252,21 +2763,21 @@
         <v>23</v>
       </c>
       <c r="G12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -2275,7 +2786,7 @@
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -2284,21 +2795,21 @@
         <v>23</v>
       </c>
       <c r="G13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="J13">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -2325,12 +2836,12 @@
         <v>10</v>
       </c>
       <c r="J14">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -2339,7 +2850,7 @@
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -2362,19 +2873,19 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="s">
         <v>23</v>
@@ -2389,24 +2900,24 @@
         <v>10</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="s">
         <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="s">
         <v>23</v>
@@ -2421,7 +2932,7 @@
         <v>10</v>
       </c>
       <c r="J17">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -2429,7 +2940,7 @@
         <v>3</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" t="s">
         <v>22</v>
@@ -2438,19 +2949,19 @@
         <v>27</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="s">
         <v>23</v>
       </c>
       <c r="G18" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="J18">
         <v>7</v>
@@ -2461,31 +2972,31 @@
         <v>3</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
         <v>23</v>
       </c>
       <c r="G19" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -2493,28 +3004,28 @@
         <v>3</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F20" t="s">
         <v>23</v>
       </c>
       <c r="G20" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -2522,49 +3033,1713 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>72</v>
+      </c>
+      <c r="J21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" t="s">
         <v>27</v>
       </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>10</v>
+      </c>
+      <c r="J22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>10</v>
+      </c>
+      <c r="J23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>10</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>10</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>72</v>
+      </c>
+      <c r="J26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>72</v>
+      </c>
+      <c r="J27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>72</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>72</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>10</v>
+      </c>
+      <c r="J30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>10</v>
+      </c>
+      <c r="J31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>10</v>
+      </c>
+      <c r="J32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>10</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>72</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>72</v>
+      </c>
+      <c r="J35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" t="s">
+        <v>25</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>72</v>
+      </c>
+      <c r="J36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>72</v>
+      </c>
+      <c r="J37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>10</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>10</v>
+      </c>
+      <c r="J39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>10</v>
+      </c>
+      <c r="J40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" t="s">
+        <v>32</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>10</v>
+      </c>
+      <c r="J41">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>72</v>
+      </c>
+      <c r="J42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" t="s">
+        <v>31</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43" t="s">
+        <v>25</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>72</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44" t="s">
+        <v>25</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>72</v>
+      </c>
+      <c r="J44">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>23</v>
+      </c>
+      <c r="G45" t="s">
+        <v>25</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>72</v>
+      </c>
+      <c r="J45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46" t="s">
+        <v>23</v>
+      </c>
+      <c r="G46" t="s">
+        <v>30</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>10</v>
+      </c>
+      <c r="J46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" t="s">
+        <v>31</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" t="s">
+        <v>30</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>10</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48" t="s">
+        <v>30</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>10</v>
+      </c>
+      <c r="J48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" t="s">
+        <v>32</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49" t="s">
+        <v>23</v>
+      </c>
+      <c r="G49" t="s">
+        <v>30</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>10</v>
+      </c>
+      <c r="J49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50" t="s">
+        <v>23</v>
+      </c>
+      <c r="G50" t="s">
+        <v>25</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>72</v>
+      </c>
+      <c r="J50">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>22</v>
+      </c>
+      <c r="D51" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51" t="s">
+        <v>23</v>
+      </c>
+      <c r="G51" t="s">
+        <v>25</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>72</v>
+      </c>
+      <c r="J51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52" t="s">
+        <v>23</v>
+      </c>
+      <c r="G52" t="s">
+        <v>25</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>72</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>22</v>
+      </c>
+      <c r="D53" t="s">
+        <v>32</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>23</v>
+      </c>
+      <c r="G53" t="s">
+        <v>25</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>72</v>
+      </c>
+      <c r="J53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54" t="s">
+        <v>23</v>
+      </c>
+      <c r="G54" t="s">
+        <v>30</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>10</v>
+      </c>
+      <c r="J54">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" t="s">
+        <v>31</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55" t="s">
+        <v>23</v>
+      </c>
+      <c r="G55" t="s">
+        <v>30</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>10</v>
+      </c>
+      <c r="J55">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>23</v>
+      </c>
+      <c r="G56" t="s">
+        <v>30</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>10</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" t="s">
+        <v>32</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57" t="s">
+        <v>23</v>
+      </c>
+      <c r="G57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>10</v>
+      </c>
+      <c r="J57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>32</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" t="s">
+        <v>27</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="F58" t="s">
+        <v>23</v>
+      </c>
+      <c r="G58" t="s">
+        <v>25</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>72</v>
+      </c>
+      <c r="J58">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>32</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" t="s">
+        <v>31</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+      <c r="F59" t="s">
+        <v>23</v>
+      </c>
+      <c r="G59" t="s">
+        <v>25</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>72</v>
+      </c>
+      <c r="J59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>32</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>22</v>
+      </c>
+      <c r="D60" t="s">
+        <v>3</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="F60" t="s">
+        <v>23</v>
+      </c>
+      <c r="G60" t="s">
+        <v>25</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>72</v>
+      </c>
+      <c r="J60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>22</v>
+      </c>
+      <c r="D61" t="s">
+        <v>32</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="F61" t="s">
+        <v>23</v>
+      </c>
+      <c r="G61" t="s">
+        <v>25</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>72</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>32</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
+      <c r="F62" t="s">
+        <v>23</v>
+      </c>
+      <c r="G62" t="s">
+        <v>30</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>10</v>
+      </c>
+      <c r="J62">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>32</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>22</v>
+      </c>
+      <c r="D63" t="s">
+        <v>31</v>
+      </c>
+      <c r="E63">
+        <v>2</v>
+      </c>
+      <c r="F63" t="s">
+        <v>23</v>
+      </c>
+      <c r="G63" t="s">
+        <v>30</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>10</v>
+      </c>
+      <c r="J63">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>32</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>22</v>
+      </c>
+      <c r="D64" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64">
+        <v>2</v>
+      </c>
+      <c r="F64" t="s">
+        <v>23</v>
+      </c>
+      <c r="G64" t="s">
+        <v>30</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>10</v>
+      </c>
+      <c r="J64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>32</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>22</v>
+      </c>
+      <c r="D65" t="s">
+        <v>32</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="F65" t="s">
+        <v>23</v>
+      </c>
+      <c r="G65" t="s">
+        <v>30</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>10</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66">
+        <v>2</v>
+      </c>
+      <c r="C66" t="s">
+        <v>22</v>
+      </c>
+      <c r="D66" t="s">
         <v>29</v>
       </c>
-      <c r="E21">
-        <v>3</v>
-      </c>
-      <c r="F21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="E66">
+        <v>3</v>
+      </c>
+      <c r="F66" t="s">
+        <v>23</v>
+      </c>
+      <c r="G66" t="s">
         <v>30</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
         <v>10</v>
       </c>
-      <c r="J21">
+      <c r="J66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>32</v>
+      </c>
+      <c r="B67">
+        <v>2</v>
+      </c>
+      <c r="C67" t="s">
+        <v>22</v>
+      </c>
+      <c r="D67" t="s">
+        <v>29</v>
+      </c>
+      <c r="E67">
+        <v>3</v>
+      </c>
+      <c r="F67" t="s">
+        <v>23</v>
+      </c>
+      <c r="G67" t="s">
+        <v>30</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>10</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>27</v>
+      </c>
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68" t="s">
+        <v>22</v>
+      </c>
+      <c r="D68" t="s">
+        <v>29</v>
+      </c>
+      <c r="E68">
+        <v>3</v>
+      </c>
+      <c r="F68" t="s">
+        <v>23</v>
+      </c>
+      <c r="G68" t="s">
+        <v>30</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>10</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69">
+        <v>2</v>
+      </c>
+      <c r="C69" t="s">
+        <v>22</v>
+      </c>
+      <c r="D69" t="s">
+        <v>29</v>
+      </c>
+      <c r="E69">
+        <v>3</v>
+      </c>
+      <c r="F69" t="s">
+        <v>23</v>
+      </c>
+      <c r="G69" t="s">
+        <v>30</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>10</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70">
+        <v>2</v>
+      </c>
+      <c r="C70" t="s">
+        <v>22</v>
+      </c>
+      <c r="D70" t="s">
+        <v>29</v>
+      </c>
+      <c r="E70">
+        <v>3</v>
+      </c>
+      <c r="F70" t="s">
+        <v>23</v>
+      </c>
+      <c r="G70" t="s">
+        <v>25</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>72</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>32</v>
+      </c>
+      <c r="B71">
+        <v>2</v>
+      </c>
+      <c r="C71" t="s">
+        <v>22</v>
+      </c>
+      <c r="D71" t="s">
+        <v>29</v>
+      </c>
+      <c r="E71">
+        <v>3</v>
+      </c>
+      <c r="F71" t="s">
+        <v>23</v>
+      </c>
+      <c r="G71" t="s">
+        <v>25</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>72</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>27</v>
+      </c>
+      <c r="B72">
+        <v>2</v>
+      </c>
+      <c r="C72" t="s">
+        <v>22</v>
+      </c>
+      <c r="D72" t="s">
+        <v>29</v>
+      </c>
+      <c r="E72">
+        <v>3</v>
+      </c>
+      <c r="F72" t="s">
+        <v>23</v>
+      </c>
+      <c r="G72" t="s">
+        <v>25</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>72</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>31</v>
+      </c>
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73" t="s">
+        <v>22</v>
+      </c>
+      <c r="D73" t="s">
+        <v>29</v>
+      </c>
+      <c r="E73">
+        <v>3</v>
+      </c>
+      <c r="F73" t="s">
+        <v>23</v>
+      </c>
+      <c r="G73" t="s">
+        <v>25</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>72</v>
+      </c>
+      <c r="J73">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J7" xr:uid="{96EB14DA-D016-4997-9091-5CA43F8416A6}"/>
+  <autoFilter ref="A1:J73" xr:uid="{96EB14DA-D016-4997-9091-5CA43F8416A6}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2573,34 +4748,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2641,7 +4816,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
@@ -2650,19 +4825,19 @@
         <v>3</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
         <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -2670,7 +4845,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2679,7 +4854,7 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2688,13 +4863,13 @@
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -2702,19 +4877,19 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
@@ -2729,6 +4904,134 @@
         <v>10</v>
       </c>
       <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>72</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>72</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>10</v>
+      </c>
+      <c r="J9">
         <v>0</v>
       </c>
     </row>
@@ -2738,13 +5041,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2753,34 +5056,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2807,10 +5110,10 @@
         <v>25</v>
       </c>
       <c r="H2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -2821,7 +5124,7 @@
         <v>27</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
@@ -2830,13 +5133,13 @@
         <v>27</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
         <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -2850,7 +5153,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2859,7 +5162,7 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2868,13 +5171,13 @@
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -2882,19 +5185,19 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
@@ -2903,12 +5206,140 @@
         <v>30</v>
       </c>
       <c r="H5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
+      </c>
+      <c r="I6">
+        <v>20</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8">
+        <v>30</v>
+      </c>
+      <c r="I8">
+        <v>30</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9">
         <v>0</v>
       </c>
     </row>
@@ -2916,248 +5347,4 @@
   <autoFilter ref="A1:J3" xr:uid="{62F394A8-9F05-4E55-93AD-A5A4A265C3A8}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:J7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="7" max="7" width="12.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2">
-        <v>12</v>
-      </c>
-      <c r="I2">
-        <v>12</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3">
-        <v>60</v>
-      </c>
-      <c r="I3">
-        <v>60</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4">
-        <v>72</v>
-      </c>
-      <c r="I4">
-        <v>72</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5">
-        <v>6</v>
-      </c>
-      <c r="I5">
-        <v>6</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6">
-        <v>4</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7">
-        <v>10</v>
-      </c>
-      <c r="I7">
-        <v>10</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:J4" xr:uid="{BCC15CB7-F490-4A4D-8BC1-B0D4AB66EEE8}"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fix subgradient max funct, add structures for greedy swap
</commit_message>
<xml_diff>
--- a/DEAS_Equipment.xlsx
+++ b/DEAS_Equipment.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronnie\Desktop\DEAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819B554B-5646-489B-9381-AE775F5D3B3A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DCB94A-FB63-4455-9113-415ABC6AA4FC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Room Inventories" sheetId="1" r:id="rId1"/>
-    <sheet name="Deployed Units" sheetId="11" r:id="rId2"/>
-    <sheet name="Commodities" sheetId="2" r:id="rId3"/>
-    <sheet name="Storage Rooms" sheetId="3" r:id="rId4"/>
-    <sheet name="Cost Data" sheetId="4" r:id="rId5"/>
-    <sheet name="Event Requirements" sheetId="6" r:id="rId6"/>
+    <sheet name="Event Requirements" sheetId="6" r:id="rId1"/>
+    <sheet name="Room Inventories" sheetId="1" r:id="rId2"/>
+    <sheet name="Deployed Units" sheetId="11" r:id="rId3"/>
+    <sheet name="Commodities" sheetId="2" r:id="rId4"/>
+    <sheet name="Storage Rooms" sheetId="3" r:id="rId5"/>
+    <sheet name="Cost Data" sheetId="4" r:id="rId6"/>
     <sheet name="Movement Arcs" sheetId="7" r:id="rId7"/>
     <sheet name="Storage Room Arcs" sheetId="8" r:id="rId8"/>
     <sheet name="Event Room Arcs" sheetId="9" r:id="rId9"/>
@@ -27,7 +27,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Event Room Arcs'!$A$1:$J$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Movement Arcs'!$A$1:$J$73</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Room Inventories'!$A$1:$C$1771</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Room Inventories'!$A$1:$C$1771</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Storage Room Arcs'!$A$1:$J$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Utility Arcs'!$A$1:$J$4</definedName>
     <definedName name="Commodities">Commodities!$A$2:$A$3</definedName>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="36">
   <si>
     <t>Storage Room</t>
   </si>
@@ -150,6 +150,12 @@
   <si>
     <t>Useful?</t>
   </si>
+  <si>
+    <t>Swap Order</t>
+  </si>
+  <si>
+    <t>ROUND</t>
+  </si>
 </sst>
 </file>
 
@@ -186,7 +192,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -339,6 +345,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -376,13 +393,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,75 +713,817 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:H129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.26953125" customWidth="1"/>
+    <col min="2" max="2" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4">
+      <c r="E1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
+      <c r="G1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+    </row>
+    <row r="66" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+    </row>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+    </row>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+    </row>
+    <row r="77" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+    </row>
+    <row r="78" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+    </row>
+    <row r="79" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+    </row>
+    <row r="80" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+    </row>
+    <row r="82" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+    </row>
+    <row r="83" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+    </row>
+    <row r="84" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+    </row>
+    <row r="85" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+    </row>
+    <row r="86" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+    </row>
+    <row r="87" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+    </row>
+    <row r="88" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+    </row>
+    <row r="89" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+    </row>
+    <row r="90" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+    </row>
+    <row r="91" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+    </row>
+    <row r="92" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+    </row>
+    <row r="93" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+    </row>
+    <row r="94" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+    </row>
+    <row r="95" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+    </row>
+    <row r="96" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+    </row>
+    <row r="97" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+    </row>
+    <row r="98" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+    </row>
+    <row r="99" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+    </row>
+    <row r="100" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+    </row>
+    <row r="101" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+    </row>
+    <row r="102" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+    </row>
+    <row r="103" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+    </row>
+    <row r="104" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+    </row>
+    <row r="105" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
+    </row>
+    <row r="106" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+    </row>
+    <row r="107" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+    </row>
+    <row r="108" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+    </row>
+    <row r="109" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+    </row>
+    <row r="110" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+    </row>
+    <row r="111" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
+    </row>
+    <row r="112" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
+    </row>
+    <row r="113" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2"/>
+    </row>
+    <row r="114" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C114" s="2"/>
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2"/>
+    </row>
+    <row r="115" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C115" s="2"/>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
+    </row>
+    <row r="116" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+    </row>
+    <row r="117" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
+    </row>
+    <row r="118" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C118" s="2"/>
+      <c r="D118" s="2"/>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
+    </row>
+    <row r="119" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C119" s="2"/>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+    </row>
+    <row r="120" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C120" s="2"/>
+      <c r="D120" s="2"/>
+      <c r="E120" s="2"/>
+      <c r="F120" s="2"/>
+    </row>
+    <row r="121" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C121" s="2"/>
+      <c r="D121" s="2"/>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2"/>
+    </row>
+    <row r="122" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C122" s="2"/>
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2"/>
+    </row>
+    <row r="123" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2"/>
+    </row>
+    <row r="124" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C124" s="2"/>
+      <c r="D124" s="2"/>
+      <c r="E124" s="2"/>
+      <c r="F124" s="2"/>
+    </row>
+    <row r="125" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C125" s="2"/>
+      <c r="D125" s="2"/>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2"/>
+    </row>
+    <row r="126" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C126" s="2"/>
+      <c r="D126" s="2"/>
+      <c r="E126" s="2"/>
+      <c r="F126" s="2"/>
+    </row>
+    <row r="127" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C127" s="2"/>
+      <c r="D127" s="2"/>
+      <c r="E127" s="2"/>
+      <c r="F127" s="2"/>
+    </row>
+    <row r="128" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C128" s="2"/>
+      <c r="D128" s="2"/>
+      <c r="E128" s="2"/>
+      <c r="F128" s="2"/>
+    </row>
+    <row r="129" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C129" s="2"/>
+      <c r="D129" s="2"/>
+      <c r="E129" s="2"/>
+      <c r="F129" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1144,26 +1903,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3400B00F-A93C-4A24-A597-B4693608C43F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1172,79 +1913,83 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>30</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
       <c r="C3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" s="3"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" s="3"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" s="3"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" s="3"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="3"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="3"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="3"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="3"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" s="3"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="3"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" s="3"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" s="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3400B00F-A93C-4A24-A597-B4693608C43F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1252,12 +1997,126 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="3"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="3"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1284,11 +2143,17 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>32</v>
+      </c>
+      <c r="B3">
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -1453,7 +2318,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -1476,10 +2341,10 @@
       <c r="B1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
@@ -1490,13 +2355,13 @@
       <c r="A2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="16">
-        <v>0</v>
-      </c>
-      <c r="C2" s="16">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
         <v>5</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2">
         <v>7</v>
       </c>
       <c r="E2" s="6">
@@ -1504,16 +2369,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3">
         <v>5</v>
       </c>
-      <c r="C3" s="16">
-        <v>0</v>
-      </c>
-      <c r="D3" s="16">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>8</v>
       </c>
       <c r="E3" s="6">
@@ -1521,16 +2386,16 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="16">
+      <c r="A4" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>7</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4">
         <v>8</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" s="6">
@@ -1553,824 +2418,6 @@
       <c r="E5" s="8">
         <v>0</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:H129"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="26.26953125" customWidth="1"/>
-    <col min="2" max="2" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-    </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-    </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-    </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-    </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-    </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-    </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-    </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-    </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-    </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-    </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-    </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-    </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-    </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-    </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-    </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-    </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-    </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-    </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-    </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
-    </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
-    </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-    </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-    </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
-    </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
-    </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
-    </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
-    </row>
-    <row r="79" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
-    </row>
-    <row r="80" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-    </row>
-    <row r="81" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-    </row>
-    <row r="82" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-    </row>
-    <row r="83" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
-      <c r="E83" s="2"/>
-      <c r="F83" s="2"/>
-    </row>
-    <row r="84" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
-    </row>
-    <row r="85" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-    </row>
-    <row r="86" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
-      <c r="E86" s="2"/>
-      <c r="F86" s="2"/>
-    </row>
-    <row r="87" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
-      <c r="E87" s="2"/>
-      <c r="F87" s="2"/>
-    </row>
-    <row r="88" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
-      <c r="E88" s="2"/>
-      <c r="F88" s="2"/>
-    </row>
-    <row r="89" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
-      <c r="F89" s="2"/>
-    </row>
-    <row r="90" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2"/>
-      <c r="F90" s="2"/>
-    </row>
-    <row r="91" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="2"/>
-      <c r="F91" s="2"/>
-    </row>
-    <row r="92" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="2"/>
-      <c r="F92" s="2"/>
-    </row>
-    <row r="93" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
-    </row>
-    <row r="94" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C94" s="2"/>
-      <c r="D94" s="2"/>
-      <c r="E94" s="2"/>
-      <c r="F94" s="2"/>
-    </row>
-    <row r="95" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
-      <c r="E95" s="2"/>
-      <c r="F95" s="2"/>
-    </row>
-    <row r="96" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
-      <c r="E96" s="2"/>
-      <c r="F96" s="2"/>
-    </row>
-    <row r="97" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
-      <c r="E97" s="2"/>
-      <c r="F97" s="2"/>
-    </row>
-    <row r="98" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
-    </row>
-    <row r="99" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
-      <c r="E99" s="2"/>
-      <c r="F99" s="2"/>
-    </row>
-    <row r="100" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-    </row>
-    <row r="101" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
-      <c r="E101" s="2"/>
-      <c r="F101" s="2"/>
-    </row>
-    <row r="102" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C102" s="2"/>
-      <c r="D102" s="2"/>
-      <c r="E102" s="2"/>
-      <c r="F102" s="2"/>
-    </row>
-    <row r="103" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C103" s="2"/>
-      <c r="D103" s="2"/>
-      <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
-    </row>
-    <row r="104" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
-      <c r="E104" s="2"/>
-      <c r="F104" s="2"/>
-    </row>
-    <row r="105" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C105" s="2"/>
-      <c r="D105" s="2"/>
-      <c r="E105" s="2"/>
-      <c r="F105" s="2"/>
-    </row>
-    <row r="106" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C106" s="2"/>
-      <c r="D106" s="2"/>
-      <c r="E106" s="2"/>
-      <c r="F106" s="2"/>
-    </row>
-    <row r="107" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C107" s="2"/>
-      <c r="D107" s="2"/>
-      <c r="E107" s="2"/>
-      <c r="F107" s="2"/>
-    </row>
-    <row r="108" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C108" s="2"/>
-      <c r="D108" s="2"/>
-      <c r="E108" s="2"/>
-      <c r="F108" s="2"/>
-    </row>
-    <row r="109" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C109" s="2"/>
-      <c r="D109" s="2"/>
-      <c r="E109" s="2"/>
-      <c r="F109" s="2"/>
-    </row>
-    <row r="110" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C110" s="2"/>
-      <c r="D110" s="2"/>
-      <c r="E110" s="2"/>
-      <c r="F110" s="2"/>
-    </row>
-    <row r="111" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C111" s="2"/>
-      <c r="D111" s="2"/>
-      <c r="E111" s="2"/>
-      <c r="F111" s="2"/>
-    </row>
-    <row r="112" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C112" s="2"/>
-      <c r="D112" s="2"/>
-      <c r="E112" s="2"/>
-      <c r="F112" s="2"/>
-    </row>
-    <row r="113" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C113" s="2"/>
-      <c r="D113" s="2"/>
-      <c r="E113" s="2"/>
-      <c r="F113" s="2"/>
-    </row>
-    <row r="114" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C114" s="2"/>
-      <c r="D114" s="2"/>
-      <c r="E114" s="2"/>
-      <c r="F114" s="2"/>
-    </row>
-    <row r="115" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C115" s="2"/>
-      <c r="D115" s="2"/>
-      <c r="E115" s="2"/>
-      <c r="F115" s="2"/>
-    </row>
-    <row r="116" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C116" s="2"/>
-      <c r="D116" s="2"/>
-      <c r="E116" s="2"/>
-      <c r="F116" s="2"/>
-    </row>
-    <row r="117" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C117" s="2"/>
-      <c r="D117" s="2"/>
-      <c r="E117" s="2"/>
-      <c r="F117" s="2"/>
-    </row>
-    <row r="118" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C118" s="2"/>
-      <c r="D118" s="2"/>
-      <c r="E118" s="2"/>
-      <c r="F118" s="2"/>
-    </row>
-    <row r="119" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C119" s="2"/>
-      <c r="D119" s="2"/>
-      <c r="E119" s="2"/>
-      <c r="F119" s="2"/>
-    </row>
-    <row r="120" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C120" s="2"/>
-      <c r="D120" s="2"/>
-      <c r="E120" s="2"/>
-      <c r="F120" s="2"/>
-    </row>
-    <row r="121" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C121" s="2"/>
-      <c r="D121" s="2"/>
-      <c r="E121" s="2"/>
-      <c r="F121" s="2"/>
-    </row>
-    <row r="122" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C122" s="2"/>
-      <c r="D122" s="2"/>
-      <c r="E122" s="2"/>
-      <c r="F122" s="2"/>
-    </row>
-    <row r="123" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C123" s="2"/>
-      <c r="D123" s="2"/>
-      <c r="E123" s="2"/>
-      <c r="F123" s="2"/>
-    </row>
-    <row r="124" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C124" s="2"/>
-      <c r="D124" s="2"/>
-      <c r="E124" s="2"/>
-      <c r="F124" s="2"/>
-    </row>
-    <row r="125" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C125" s="2"/>
-      <c r="D125" s="2"/>
-      <c r="E125" s="2"/>
-      <c r="F125" s="2"/>
-    </row>
-    <row r="126" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C126" s="2"/>
-      <c r="D126" s="2"/>
-      <c r="E126" s="2"/>
-      <c r="F126" s="2"/>
-    </row>
-    <row r="127" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C127" s="2"/>
-      <c r="D127" s="2"/>
-      <c r="E127" s="2"/>
-      <c r="F127" s="2"/>
-    </row>
-    <row r="128" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C128" s="2"/>
-      <c r="D128" s="2"/>
-      <c r="E128" s="2"/>
-      <c r="F128" s="2"/>
-    </row>
-    <row r="129" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C129" s="2"/>
-      <c r="D129" s="2"/>
-      <c r="E129" s="2"/>
-      <c r="F129" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added two more superevents
</commit_message>
<xml_diff>
--- a/DEAS_Equipment.xlsx
+++ b/DEAS_Equipment.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="1" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="10420" windowWidth="19420" xWindow="-110" yWindow="-110"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="10420" windowWidth="19420" xWindow="-110" yWindow="-110"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Event Requirements" sheetId="1" state="visible" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <definedName name="Rooms">'Cost Data'!#REF!</definedName>
     <definedName name="StorageRooms">'Storage Rooms'!$A$2:$A$3</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>Event</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>ER3</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>Chairs</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
   </si>
   <si>
     <t>Storage Room</t>
@@ -157,8 +169,8 @@
   <numFmts count="4">
     <numFmt formatCode="yyyy\-mm\-dd\ hh:mm:ss" numFmtId="164"/>
     <numFmt formatCode="[$-F400]h:mm:ss\ AM/PM" numFmtId="165"/>
-    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="166"/>
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="167"/>
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="166"/>
+    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="167"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -455,9 +467,9 @@
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="14" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="15" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="13" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="13" fillId="3" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -769,9 +781,9 @@
   </sheetPr>
   <dimension ref="A1:H129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="F17" pane="bottomLeft" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A10" ySplit="1"/>
+      <selection activeCell="A20" pane="bottomLeft" sqref="A20:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -1071,87 +1083,291 @@
         <v>5</v>
       </c>
     </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="18" t="n">
+        <v>43559.5</v>
+      </c>
+      <c r="D12" s="18" t="n">
+        <v>43559.54166666666</v>
+      </c>
+      <c r="E12" s="18" t="n">
+        <v>43559.58333333334</v>
+      </c>
+      <c r="F12" s="18" t="n">
+        <v>43559.625</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="22" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="31" t="n">
+        <v>43560.04166666666</v>
+      </c>
+      <c r="D13" s="31" t="n">
+        <v>43560.08333333334</v>
+      </c>
+      <c r="E13" s="31" t="n">
+        <v>43560.125</v>
+      </c>
+      <c r="F13" s="31" t="n">
+        <v>43560.16666666666</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="30" t="n">
+        <v>40</v>
+      </c>
+    </row>
     <row r="14" spans="1:8">
-      <c r="C14" s="30" t="n"/>
-      <c r="D14" s="30" t="n"/>
+      <c r="A14" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="31" t="n">
+        <v>43560.04166666666</v>
+      </c>
+      <c r="D14" s="31" t="n">
+        <v>43560.08333333334</v>
+      </c>
+      <c r="E14" s="31" t="n">
+        <v>43560.125</v>
+      </c>
+      <c r="F14" s="31" t="n">
+        <v>43560.16666666666</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="19" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="31" t="n">
+        <v>43560.04166666666</v>
+      </c>
+      <c r="D15" s="31" t="n">
+        <v>43560.08333333334</v>
+      </c>
+      <c r="E15" s="31" t="n">
+        <v>43560.125</v>
+      </c>
+      <c r="F15" s="31" t="n">
+        <v>43560.16666666666</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="19" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="31" t="n">
+        <v>43560.04166666666</v>
+      </c>
+      <c r="D16" s="31" t="n">
+        <v>43560.08333333334</v>
+      </c>
+      <c r="E16" s="31" t="n">
+        <v>43560.125</v>
+      </c>
+      <c r="F16" s="31" t="n">
+        <v>43560.16666666666</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="19" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="20" t="n">
+        <v>43560.25</v>
+      </c>
+      <c r="D17" s="20" t="n">
+        <v>43560.29166666666</v>
+      </c>
+      <c r="E17" s="20" t="n">
+        <v>43560.33333333334</v>
+      </c>
+      <c r="F17" s="20" t="n">
+        <v>43560.375</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="19" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="20" t="n">
+        <v>43560.25</v>
+      </c>
+      <c r="D18" s="20" t="n">
+        <v>43560.29166666666</v>
+      </c>
+      <c r="E18" s="20" t="n">
+        <v>43560.33333333334</v>
+      </c>
+      <c r="F18" s="20" t="n">
+        <v>43560.375</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="19" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="18" t="n">
+        <v>43560.20833333334</v>
+      </c>
+      <c r="D19" s="18" t="n">
+        <v>43560.25</v>
+      </c>
+      <c r="E19" s="18" t="n">
+        <v>43560.29166666666</v>
+      </c>
+      <c r="F19" s="18" t="n">
+        <v>43560.33333333334</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="17" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="C20" s="2" t="n"/>
-      <c r="D20" s="2" t="n"/>
-      <c r="E20" s="2" t="n"/>
-      <c r="F20" s="2" t="n"/>
+      <c r="A20" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="18" t="n">
+        <v>43560.20833333334</v>
+      </c>
+      <c r="D20" s="18" t="n">
+        <v>43560.25</v>
+      </c>
+      <c r="E20" s="18" t="n">
+        <v>43560.29166666666</v>
+      </c>
+      <c r="F20" s="18" t="n">
+        <v>43560.33333333334</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="17" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="C21" s="2" t="n"/>
-      <c r="D21" s="2" t="n"/>
-      <c r="E21" s="2" t="n"/>
-      <c r="F21" s="2" t="n"/>
+      <c r="A21" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="18" t="n">
+        <v>43560.29166666666</v>
+      </c>
+      <c r="D21" s="18" t="n">
+        <v>43560.33333333334</v>
+      </c>
+      <c r="E21" s="18" t="n">
+        <v>43560.375</v>
+      </c>
+      <c r="F21" s="18" t="n">
+        <v>43560.41666666666</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="17" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="C22" s="2" t="n"/>
-      <c r="D22" s="2" t="n"/>
-      <c r="E22" s="2" t="n"/>
-      <c r="F22" s="2" t="n"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="C23" s="2" t="n"/>
-      <c r="D23" s="2" t="n"/>
-      <c r="E23" s="2" t="n"/>
-      <c r="F23" s="2" t="n"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="C24" s="2" t="n"/>
-      <c r="D24" s="2" t="n"/>
-      <c r="E24" s="2" t="n"/>
-      <c r="F24" s="2" t="n"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="C25" s="2" t="n"/>
-      <c r="D25" s="2" t="n"/>
-      <c r="E25" s="2" t="n"/>
-      <c r="F25" s="2" t="n"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="C26" s="2" t="n"/>
-      <c r="D26" s="2" t="n"/>
-      <c r="E26" s="2" t="n"/>
-      <c r="F26" s="2" t="n"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="C27" s="2" t="n"/>
-      <c r="D27" s="2" t="n"/>
-      <c r="E27" s="2" t="n"/>
-      <c r="F27" s="2" t="n"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="C28" s="2" t="n"/>
-      <c r="D28" s="2" t="n"/>
-      <c r="E28" s="2" t="n"/>
-      <c r="F28" s="2" t="n"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="C29" s="2" t="n"/>
-      <c r="D29" s="2" t="n"/>
-      <c r="E29" s="2" t="n"/>
-      <c r="F29" s="2" t="n"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="C30" s="2" t="n"/>
-      <c r="D30" s="2" t="n"/>
-      <c r="E30" s="2" t="n"/>
-      <c r="F30" s="2" t="n"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="C31" s="2" t="n"/>
-      <c r="D31" s="2" t="n"/>
-      <c r="E31" s="2" t="n"/>
-      <c r="F31" s="2" t="n"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="C32" s="2" t="n"/>
-      <c r="D32" s="2" t="n"/>
-      <c r="E32" s="2" t="n"/>
-      <c r="F32" s="2" t="n"/>
+      <c r="A22" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="18" t="n">
+        <v>43560.29166666666</v>
+      </c>
+      <c r="D22" s="18" t="n">
+        <v>43560.33333333334</v>
+      </c>
+      <c r="E22" s="18" t="n">
+        <v>43560.375</v>
+      </c>
+      <c r="F22" s="18" t="n">
+        <v>43560.41666666666</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="17" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
       <c r="C33" s="2" t="n"/>
@@ -1763,10 +1979,10 @@
   <sheetData>
     <row customHeight="1" ht="15" r="1" spans="1:3" thickBot="1">
       <c r="A1" s="24" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C1" s="26" t="s">
         <v>7</v>
@@ -1774,7 +1990,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -1785,7 +2001,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -1796,7 +2012,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -1807,7 +2023,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -1818,7 +2034,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -1829,7 +2045,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -1863,10 +2079,10 @@
   <sheetData>
     <row customHeight="1" ht="15" r="1" spans="1:3" thickBot="1">
       <c r="A1" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>16</v>
       </c>
       <c r="C1" s="26" t="s">
         <v>7</v>
@@ -1874,7 +2090,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1890,9 +2106,9 @@
   </sheetPr>
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="C7" pane="bottomLeft" sqref="C7"/>
+      <selection activeCell="B1" pane="bottomLeft" sqref="B1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -1906,19 +2122,19 @@
   <sheetData>
     <row customHeight="1" ht="15" r="1" spans="1:6" thickBot="1">
       <c r="A1" s="24" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row customHeight="1" ht="17" r="2" spans="1:6">
@@ -1957,7 +2173,7 @@
     </row>
     <row customHeight="1" ht="15" r="4" spans="1:6" thickBot="1">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B4" t="n">
         <v>2</v>
@@ -2040,63 +2256,63 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="n"/>
       <c r="D2" t="n">
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="n"/>
       <c r="D3" t="n">
         <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D4" t="n">
         <v>50</v>
@@ -2297,13 +2513,13 @@
         <v>14</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2377,7 +2593,7 @@
     </row>
     <row customHeight="1" ht="15" r="5" spans="1:7">
       <c r="A5" s="14" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B5" t="n">
         <v>7</v>
@@ -2400,7 +2616,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="14" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B6" t="n">
         <v>9</v>
@@ -2423,7 +2639,7 @@
     </row>
     <row customHeight="1" ht="15" r="7" spans="1:7" thickBot="1">
       <c r="A7" s="13" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>10</v>
@@ -2455,7 +2671,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2468,19 +2684,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2488,7 +2704,7 @@
         <v>43559.04166666666</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -2505,16 +2721,16 @@
         <v>43559.04166666666</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2522,7 +2738,7 @@
         <v>43559.04166666666</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -2539,7 +2755,7 @@
         <v>43559.04166666666</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -2556,7 +2772,7 @@
         <v>43559.04166666666</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -2570,36 +2786,36 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="32" t="n">
-        <v>43559.25</v>
+        <v>43559.04166666666</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="32" t="n">
-        <v>43559.25</v>
+        <v>43559.04166666666</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2607,16 +2823,16 @@
         <v>43559.25</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>30</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2624,84 +2840,84 @@
         <v>43559.25</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="32" t="n">
-        <v>43559.20833333334</v>
+        <v>43559.25</v>
       </c>
       <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E11" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="32" t="n">
-        <v>43559.20833333334</v>
+        <v>43559.25</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="32" t="n">
-        <v>43559.20833333334</v>
+        <v>43559.25</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="32" t="n">
-        <v>43559.20833333334</v>
+        <v>43559.25</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2709,100 +2925,627 @@
         <v>43559.20833333334</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="32" t="n">
-        <v>43559.29166666666</v>
+        <v>43559.20833333334</v>
       </c>
       <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E16" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="32" t="n">
-        <v>43559.29166666666</v>
+        <v>43559.20833333334</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="32" t="n">
-        <v>43559.29166666666</v>
+        <v>43559.20833333334</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="32" t="n">
-        <v>43559.29166666666</v>
+        <v>43559.20833333334</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="32" t="n">
+        <v>43559.20833333334</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="32" t="n">
         <v>43559.29166666666</v>
       </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
         <v>14</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="32" t="n">
+        <v>43559.29166666666</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s">
         <v>11</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E22" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="32" t="n">
+        <v>43559.29166666666</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="32" t="n">
+        <v>43559.29166666666</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="32" t="n">
+        <v>43559.29166666666</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="32" t="n">
+        <v>43559.29166666666</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="32" t="n">
+        <v>43559.5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="32" t="n">
+        <v>43559.5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="32" t="n">
+        <v>43559.5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="32" t="n">
+        <v>43559.5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="32" t="n">
+        <v>43559.5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="32" t="n">
+        <v>43560.04166666666</v>
+      </c>
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="32" t="n">
+        <v>43560.04166666666</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="32" t="n">
+        <v>43560.04166666666</v>
+      </c>
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="32" t="n">
+        <v>43560.04166666666</v>
+      </c>
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="32" t="n">
+        <v>43560.04166666666</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="32" t="n">
+        <v>43560.04166666666</v>
+      </c>
+      <c r="B37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="32" t="n">
+        <v>43560.25</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="32" t="n">
+        <v>43560.25</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="32" t="n">
+        <v>43560.25</v>
+      </c>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="32" t="n">
+        <v>43560.25</v>
+      </c>
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="32" t="n">
+        <v>43560.20833333334</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="32" t="n">
+        <v>43560.20833333334</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="32" t="n">
+        <v>43560.20833333334</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="32" t="n">
+        <v>43560.20833333334</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="32" t="n">
+        <v>43560.20833333334</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="32" t="n">
+        <v>43560.20833333334</v>
+      </c>
+      <c r="B47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="32" t="n">
+        <v>43560.29166666666</v>
+      </c>
+      <c r="B48" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="32" t="n">
+        <v>43560.29166666666</v>
+      </c>
+      <c r="B49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="32" t="n">
+        <v>43560.29166666666</v>
+      </c>
+      <c r="B50" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="32" t="n">
+        <v>43560.29166666666</v>
+      </c>
+      <c r="B51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Outer works for DEAS_eqip. finalized structs to pass in start and end states for inner.
</commit_message>
<xml_diff>
--- a/DEAS_Equipment.xlsx
+++ b/DEAS_Equipment.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="3" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="10420" windowWidth="19420" xWindow="-110" yWindow="-110"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="10420" windowWidth="19420" xWindow="-110" yWindow="-110"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Event Requirements" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,17 +15,24 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Schedule" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'Inventory by Room'!$A$1:$C$1771</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Event Requirements'!$A$1:$H$1</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'Inventory by Room'!$A$1:$C$1</definedName>
     <definedName name="Commodities">Commodities!$A$2:$A$3</definedName>
     <definedName name="Rooms">'Cost Data'!#REF!</definedName>
     <definedName name="StorageRooms">'Storage Rooms'!$A$2:$A$3</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Event Requirements'!$A$1:$H$1</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'Inventory by Room'!$A$1:$C$1</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Event Requirements'!$A$1:$H$1</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'Inventory by Room'!$A$1:$C$1</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Event Requirements'!$A$1:$H$1</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'Inventory by Room'!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>Event</t>
   </si>
@@ -148,6 +155,9 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>echelon</t>
   </si>
   <si>
     <t>From Room</t>
@@ -163,11 +173,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt formatCode="yyyy\-mm\-dd\ hh:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="[$-F400]h:mm:ss\ AM/PM" numFmtId="165"/>
-    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="166"/>
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="167"/>
+  <numFmts count="3">
+    <numFmt formatCode="[$-F400]h:mm:ss\ AM/PM" numFmtId="164"/>
+    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="166"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -391,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -424,25 +433,27 @@
     <xf applyAlignment="1" borderId="11" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="2" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="2" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="3" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="3" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="12" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="13" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="13" fillId="2" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="13" fillId="2" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="12" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="7" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="13" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="13" fillId="3" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="13" fillId="3" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="13" fillId="2" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="2" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="3" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="13" fillId="3" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -754,24 +765,25 @@
   </sheetPr>
   <dimension ref="A1:H129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A10" ySplit="1"/>
-      <selection activeCell="A20" pane="bottomLeft" sqref="A20:A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="C6" pane="bottomLeft" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="30" width="26.26953125"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="30" width="5.7265625"/>
-    <col customWidth="1" max="3" min="3" style="30" width="26.1796875"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="30" width="13.54296875"/>
-    <col bestFit="1" customWidth="1" max="6" min="5" style="30" width="14.54296875"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="30" width="21.453125"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="30" width="8"/>
+    <col customWidth="1" max="1" min="1" width="20.26953125"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="10.26953125"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" width="15.36328125"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="14.453125"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" width="14.6328125"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" width="13.7265625"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" width="19.08984375"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" width="12.7265625"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="30" spans="1:8" thickBot="1">
-      <c r="A1" s="21" t="s">
+    <row customHeight="1" ht="15" r="1" spans="1:8" thickBot="1">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
@@ -797,548 +809,548 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="23" t="n">
+      <c r="C2" s="29" t="n">
         <v>43559.04166666666</v>
       </c>
-      <c r="D2" s="23" t="n">
+      <c r="D2" s="29" t="n">
         <v>43559.08333333334</v>
       </c>
-      <c r="E2" s="23" t="n">
+      <c r="E2" s="29" t="n">
         <v>43559.125</v>
       </c>
-      <c r="F2" s="23" t="n">
+      <c r="F2" s="29" t="n">
         <v>43559.16666666666</v>
       </c>
-      <c r="G2" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="22" t="n">
+      <c r="G2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="21" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="18" t="n">
+      <c r="C3" s="30" t="n">
         <v>43559.04166666666</v>
       </c>
-      <c r="D3" s="18" t="n">
+      <c r="D3" s="30" t="n">
         <v>43559.08333333334</v>
       </c>
-      <c r="E3" s="18" t="n">
+      <c r="E3" s="30" t="n">
         <v>43559.125</v>
       </c>
-      <c r="F3" s="18" t="n">
+      <c r="F3" s="30" t="n">
         <v>43559.16666666666</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="17" t="n">
+      <c r="H3" s="16" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="18" t="n">
+      <c r="C4" s="30" t="n">
         <v>43559.04166666666</v>
       </c>
-      <c r="D4" s="18" t="n">
+      <c r="D4" s="30" t="n">
         <v>43559.08333333334</v>
       </c>
-      <c r="E4" s="18" t="n">
+      <c r="E4" s="30" t="n">
         <v>43559.125</v>
       </c>
-      <c r="F4" s="18" t="n">
+      <c r="F4" s="30" t="n">
         <v>43559.16666666666</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="17" t="n">
+      <c r="G4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="16" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="18" t="n">
+      <c r="C5" s="30" t="n">
         <v>43559.04166666666</v>
       </c>
-      <c r="D5" s="18" t="n">
+      <c r="D5" s="30" t="n">
         <v>43559.08333333334</v>
       </c>
-      <c r="E5" s="18" t="n">
+      <c r="E5" s="30" t="n">
         <v>43559.125</v>
       </c>
-      <c r="F5" s="18" t="n">
+      <c r="F5" s="30" t="n">
         <v>43559.16666666666</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="17" t="n">
+      <c r="H5" s="16" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="18" t="n">
+      <c r="C6" s="30" t="n">
         <v>43559.25</v>
       </c>
-      <c r="D6" s="18" t="n">
+      <c r="D6" s="30" t="n">
         <v>43559.29166666666</v>
       </c>
-      <c r="E6" s="18" t="n">
+      <c r="E6" s="30" t="n">
         <v>43559.33333333334</v>
       </c>
-      <c r="F6" s="18" t="n">
+      <c r="F6" s="30" t="n">
         <v>43559.375</v>
       </c>
-      <c r="G6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="17" t="n">
+      <c r="G6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="16" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="18" t="n">
+      <c r="C7" s="30" t="n">
         <v>43559.25</v>
       </c>
-      <c r="D7" s="18" t="n">
+      <c r="D7" s="30" t="n">
         <v>43559.29166666666</v>
       </c>
-      <c r="E7" s="18" t="n">
+      <c r="E7" s="30" t="n">
         <v>43559.33333333334</v>
       </c>
-      <c r="F7" s="18" t="n">
+      <c r="F7" s="30" t="n">
         <v>43559.375</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="17" t="n">
+      <c r="H7" s="16" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="20" t="n">
+      <c r="C8" s="31" t="n">
         <v>43559.20833333334</v>
       </c>
-      <c r="D8" s="20" t="n">
+      <c r="D8" s="31" t="n">
         <v>43559.25</v>
       </c>
-      <c r="E8" s="20" t="n">
+      <c r="E8" s="31" t="n">
         <v>43559.29166666666</v>
       </c>
-      <c r="F8" s="20" t="n">
+      <c r="F8" s="31" t="n">
         <v>43559.33333333334</v>
       </c>
-      <c r="G8" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="19" t="n">
+      <c r="G8" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="18" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="20" t="n">
+      <c r="C9" s="31" t="n">
         <v>43559.20833333334</v>
       </c>
-      <c r="D9" s="20" t="n">
+      <c r="D9" s="31" t="n">
         <v>43559.25</v>
       </c>
-      <c r="E9" s="20" t="n">
+      <c r="E9" s="31" t="n">
         <v>43559.29166666666</v>
       </c>
-      <c r="F9" s="20" t="n">
+      <c r="F9" s="31" t="n">
         <v>43559.33333333334</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="19" t="n">
+      <c r="H9" s="18" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="20" t="n">
+      <c r="C10" s="31" t="n">
         <v>43559.29166666666</v>
       </c>
-      <c r="D10" s="20" t="n">
+      <c r="D10" s="31" t="n">
         <v>43559.33333333334</v>
       </c>
-      <c r="E10" s="20" t="n">
+      <c r="E10" s="31" t="n">
         <v>43559.375</v>
       </c>
-      <c r="F10" s="20" t="n">
+      <c r="F10" s="31" t="n">
         <v>43559.41666666666</v>
       </c>
-      <c r="G10" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="19" t="n">
+      <c r="G10" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="18" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="20" t="n">
+      <c r="C11" s="31" t="n">
         <v>43559.29166666666</v>
       </c>
-      <c r="D11" s="20" t="n">
+      <c r="D11" s="31" t="n">
         <v>43559.33333333334</v>
       </c>
-      <c r="E11" s="20" t="n">
+      <c r="E11" s="31" t="n">
         <v>43559.375</v>
       </c>
-      <c r="F11" s="20" t="n">
+      <c r="F11" s="31" t="n">
         <v>43559.41666666666</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="19" t="n">
+      <c r="H11" s="18" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="n">
+      <c r="C12" s="30" t="n">
         <v>43559.5</v>
       </c>
-      <c r="D12" s="18" t="n">
+      <c r="D12" s="30" t="n">
         <v>43559.54166666666</v>
       </c>
-      <c r="E12" s="18" t="n">
+      <c r="E12" s="30" t="n">
         <v>43559.58333333334</v>
       </c>
-      <c r="F12" s="18" t="n">
+      <c r="F12" s="30" t="n">
         <v>43559.625</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="22" t="n">
+      <c r="H12" s="21" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="29" t="n">
+      <c r="C13" s="32" t="n">
         <v>43560.04166666666</v>
       </c>
-      <c r="D13" s="29" t="n">
+      <c r="D13" s="32" t="n">
         <v>43560.08333333334</v>
       </c>
-      <c r="E13" s="29" t="n">
+      <c r="E13" s="32" t="n">
         <v>43560.125</v>
       </c>
-      <c r="F13" s="29" t="n">
+      <c r="F13" s="32" t="n">
         <v>43560.16666666666</v>
       </c>
-      <c r="G13" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="28" t="n">
+      <c r="G13" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="27" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="29" t="n">
+      <c r="C14" s="32" t="n">
         <v>43560.04166666666</v>
       </c>
-      <c r="D14" s="29" t="n">
+      <c r="D14" s="32" t="n">
         <v>43560.08333333334</v>
       </c>
-      <c r="E14" s="29" t="n">
+      <c r="E14" s="32" t="n">
         <v>43560.125</v>
       </c>
-      <c r="F14" s="29" t="n">
+      <c r="F14" s="32" t="n">
         <v>43560.16666666666</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="19" t="n">
+      <c r="H14" s="18" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="29" t="n">
+      <c r="C15" s="32" t="n">
         <v>43560.04166666666</v>
       </c>
-      <c r="D15" s="29" t="n">
+      <c r="D15" s="32" t="n">
         <v>43560.08333333334</v>
       </c>
-      <c r="E15" s="29" t="n">
+      <c r="E15" s="32" t="n">
         <v>43560.125</v>
       </c>
-      <c r="F15" s="29" t="n">
+      <c r="F15" s="32" t="n">
         <v>43560.16666666666</v>
       </c>
-      <c r="G15" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="19" t="n">
+      <c r="G15" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="18" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="29" t="n">
+      <c r="C16" s="32" t="n">
         <v>43560.04166666666</v>
       </c>
-      <c r="D16" s="29" t="n">
+      <c r="D16" s="32" t="n">
         <v>43560.08333333334</v>
       </c>
-      <c r="E16" s="29" t="n">
+      <c r="E16" s="32" t="n">
         <v>43560.125</v>
       </c>
-      <c r="F16" s="29" t="n">
+      <c r="F16" s="32" t="n">
         <v>43560.16666666666</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="19" t="n">
+      <c r="H16" s="18" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="20" t="n">
+      <c r="C17" s="31" t="n">
         <v>43560.25</v>
       </c>
-      <c r="D17" s="20" t="n">
+      <c r="D17" s="31" t="n">
         <v>43560.29166666666</v>
       </c>
-      <c r="E17" s="20" t="n">
+      <c r="E17" s="31" t="n">
         <v>43560.33333333334</v>
       </c>
-      <c r="F17" s="20" t="n">
+      <c r="F17" s="31" t="n">
         <v>43560.375</v>
       </c>
-      <c r="G17" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="19" t="n">
+      <c r="G17" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="18" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="20" t="n">
+      <c r="C18" s="31" t="n">
         <v>43560.25</v>
       </c>
-      <c r="D18" s="20" t="n">
+      <c r="D18" s="31" t="n">
         <v>43560.29166666666</v>
       </c>
-      <c r="E18" s="20" t="n">
+      <c r="E18" s="31" t="n">
         <v>43560.33333333334</v>
       </c>
-      <c r="F18" s="20" t="n">
+      <c r="F18" s="31" t="n">
         <v>43560.375</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="19" t="n">
+      <c r="H18" s="18" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="18" t="n">
+      <c r="C19" s="30" t="n">
         <v>43560.20833333334</v>
       </c>
-      <c r="D19" s="18" t="n">
+      <c r="D19" s="30" t="n">
         <v>43560.25</v>
       </c>
-      <c r="E19" s="18" t="n">
+      <c r="E19" s="30" t="n">
         <v>43560.29166666666</v>
       </c>
-      <c r="F19" s="18" t="n">
+      <c r="F19" s="30" t="n">
         <v>43560.33333333334</v>
       </c>
-      <c r="G19" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="17" t="n">
+      <c r="G19" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="16" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="18" t="n">
+      <c r="C20" s="30" t="n">
         <v>43560.20833333334</v>
       </c>
-      <c r="D20" s="18" t="n">
+      <c r="D20" s="30" t="n">
         <v>43560.25</v>
       </c>
-      <c r="E20" s="18" t="n">
+      <c r="E20" s="30" t="n">
         <v>43560.29166666666</v>
       </c>
-      <c r="F20" s="18" t="n">
+      <c r="F20" s="30" t="n">
         <v>43560.33333333334</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="17" t="n">
+      <c r="H20" s="16" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="18" t="n">
+      <c r="C21" s="30" t="n">
         <v>43560.29166666666</v>
       </c>
-      <c r="D21" s="18" t="n">
+      <c r="D21" s="30" t="n">
         <v>43560.33333333334</v>
       </c>
-      <c r="E21" s="18" t="n">
+      <c r="E21" s="30" t="n">
         <v>43560.375</v>
       </c>
-      <c r="F21" s="18" t="n">
+      <c r="F21" s="30" t="n">
         <v>43560.41666666666</v>
       </c>
-      <c r="G21" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="17" t="n">
+      <c r="G21" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="16" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="18" t="n">
+      <c r="C22" s="30" t="n">
         <v>43560.29166666666</v>
       </c>
-      <c r="D22" s="18" t="n">
+      <c r="D22" s="30" t="n">
         <v>43560.33333333334</v>
       </c>
-      <c r="E22" s="18" t="n">
+      <c r="E22" s="30" t="n">
         <v>43560.375</v>
       </c>
-      <c r="F22" s="18" t="n">
+      <c r="F22" s="30" t="n">
         <v>43560.41666666666</v>
       </c>
-      <c r="G22" s="17" t="s">
+      <c r="G22" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="17" t="n">
+      <c r="H22" s="16" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1925,6 +1937,7 @@
       <c r="F129" s="2" t="n"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H1"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -1940,24 +1953,24 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="D12" pane="bottomLeft" sqref="D12"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="30" width="12.54296875"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="30" width="10.54296875"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="30" width="8.1796875"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="14.81640625"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="12.81640625"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" width="10.453125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="30" spans="1:3" thickBot="1">
-      <c r="A1" s="24" t="s">
+    <row customHeight="1" ht="15" r="1" spans="1:3" thickBot="1">
+      <c r="A1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2028,6 +2041,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -2046,18 +2060,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="30" width="16.36328125"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="30" width="10.54296875"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="16.36328125"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="10.54296875"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="30" spans="1:3" thickBot="1">
-      <c r="A1" s="24" t="s">
+    <row customHeight="1" ht="15" r="1" spans="1:3" thickBot="1">
+      <c r="A1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2079,35 +2093,35 @@
   </sheetPr>
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="D6" pane="bottomLeft" sqref="D6"/>
+      <selection activeCell="D17" pane="bottomLeft" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="30" width="10.54296875"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="30" width="12"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="30" width="18.36328125"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="30" width="10.6328125"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="30" width="12"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="10.54296875"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="12"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" width="18.36328125"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="10.6328125"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" width="12"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="30" spans="1:4" thickBot="1">
-      <c r="A1" s="24" t="s">
+    <row customHeight="1" ht="15" r="1" spans="1:4" thickBot="1">
+      <c r="A1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="2" s="30" spans="1:4">
+    <row customHeight="1" ht="17" r="2" spans="1:4">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2121,7 +2135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="3" s="30" spans="1:4">
+    <row customHeight="1" ht="17" r="3" spans="1:4">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2135,7 +2149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="4" s="30" spans="1:4">
+    <row customHeight="1" ht="15" r="4" spans="1:4">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -2205,14 +2219,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="30" width="12.54296875"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="30" width="20.6328125"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="30" width="13.453125"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="30" width="20.36328125"/>
-    <col customWidth="1" max="5" min="5" style="30" width="20.36328125"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="30" width="13.1796875"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="30" width="16.453125"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="30" width="16.81640625"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="12.54296875"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="20.6328125"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" width="13.453125"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="20.36328125"/>
+    <col customWidth="1" max="5" min="5" width="20.36328125"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" width="13.1796875"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" width="16.453125"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" width="16.81640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2452,7 +2466,7 @@
       <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
       <selection activeCell="B1" pane="topRight" sqref="B1"/>
       <selection activeCell="A2" pane="bottomLeft" sqref="A2"/>
-      <selection activeCell="C11" pane="bottomRight" sqref="C11"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="10.81640625" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -2460,7 +2474,7 @@
     <col customWidth="1" max="1" min="1" style="5" width="10.81640625"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="30" spans="1:7" thickBot="1">
+    <row customHeight="1" ht="15" r="1" spans="1:7" thickBot="1">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -2552,7 +2566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="5" s="30" spans="1:7">
+    <row customHeight="1" ht="15" r="5" spans="1:7">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -2598,7 +2612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="7" s="30" spans="1:7" thickBot="1">
+    <row customHeight="1" ht="15" r="7" spans="1:7" thickBot="1">
       <c r="A7" s="13" t="s">
         <v>23</v>
       </c>
@@ -2632,18 +2646,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
-  <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="30" width="17.81640625"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -2654,1539 +2665,612 @@
         <v>42</v>
       </c>
       <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="32" t="n">
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="34" t="n">
         <v>43559.04166666666</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="32" t="n">
+    <row r="3" spans="1:6">
+      <c r="A3" s="34" t="n">
         <v>43559.04166666666</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="32" t="n">
+    <row r="4" spans="1:6">
+      <c r="A4" s="34" t="n">
         <v>43559.04166666666</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="32" t="n">
+    <row r="5" spans="1:6">
+      <c r="A5" s="34" t="n">
         <v>43559.04166666666</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="n">
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="n">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="32" t="n">
+    <row r="6" spans="1:6">
+      <c r="A6" s="34" t="n">
         <v>43559.04166666666</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="32" t="n">
+    <row r="7" spans="1:6">
+      <c r="A7" s="34" t="n">
         <v>43559.04166666666</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="n">
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="32" t="n">
+    <row r="8" spans="1:6">
+      <c r="A8" s="34" t="n">
         <v>43559.04166666666</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="32" t="n">
+    <row r="9" spans="1:6">
+      <c r="A9" s="34" t="n">
         <v>43559.41666666666</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="n">
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="32" t="n">
+    <row r="10" spans="1:6">
+      <c r="A10" s="34" t="n">
         <v>43559.41666666666</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" t="n">
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="32" t="n">
+    <row r="11" spans="1:6">
+      <c r="A11" s="34" t="n">
         <v>43559.41666666666</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>11</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="32" t="n">
+    <row r="12" spans="1:6">
+      <c r="A12" s="34" t="n">
         <v>43559.41666666666</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" t="n">
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="32" t="n">
+    <row r="13" spans="1:6">
+      <c r="A13" s="34" t="n">
         <v>43559.41666666666</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>23</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>11</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="32" t="n">
+    <row r="14" spans="1:6">
+      <c r="A14" s="34" t="n">
         <v>43559.41666666666</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>23</v>
       </c>
-      <c r="D14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" t="n">
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="32" t="n">
+    <row r="15" spans="1:6">
+      <c r="A15" s="34" t="n">
         <v>43559.41666666666</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>23</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>11</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="32" t="n">
+    <row r="16" spans="1:6">
+      <c r="A16" s="34" t="n">
         <v>43559.41666666666</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
         <v>21</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>23</v>
       </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" t="n">
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="32" t="n">
+    <row r="17" spans="1:6">
+      <c r="A17" s="34" t="n">
         <v>43559.5</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
         <v>21</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>22</v>
       </c>
-      <c r="D17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" t="n">
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="n">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="32" t="n">
+    <row r="18" spans="1:6">
+      <c r="A18" s="34" t="n">
         <v>43559.625</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
         <v>21</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>22</v>
       </c>
-      <c r="D18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" t="n">
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="n">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="32" t="n">
+    <row r="19" spans="1:6">
+      <c r="A19" s="34" t="n">
         <v>43560.04166666666</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" t="n">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
         <v>21</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>9</v>
       </c>
-      <c r="D19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" t="n">
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="32" t="n">
+    <row r="20" spans="1:6">
+      <c r="A20" s="34" t="n">
         <v>43560.04166666666</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" t="n">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
         <v>22</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>12</v>
       </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" t="n">
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="32" t="n">
+    <row r="21" spans="1:6">
+      <c r="A21" s="34" t="n">
         <v>43560.04166666666</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" t="n">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
         <v>23</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>9</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>11</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="32" t="n">
+    <row r="22" spans="1:6">
+      <c r="A22" s="34" t="n">
         <v>43560.04166666666</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" t="n">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
         <v>23</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>12</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>11</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="32" t="n">
+    <row r="23" spans="1:6">
+      <c r="A23" s="34" t="n">
         <v>43560.04166666666</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" t="n">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
         <v>23</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>14</v>
       </c>
-      <c r="D23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" t="n">
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="32" t="n">
+    <row r="24" spans="1:6">
+      <c r="A24" s="34" t="n">
         <v>43560.04166666666</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" t="n">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
         <v>23</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>14</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>11</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="32" t="n">
+    <row r="25" spans="1:6">
+      <c r="A25" s="34" t="n">
         <v>43560.41666666666</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" t="n">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
         <v>9</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>21</v>
       </c>
-      <c r="D25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" t="n">
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="32" t="n">
+    <row r="26" spans="1:6">
+      <c r="A26" s="34" t="n">
         <v>43560.41666666666</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" t="n">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
         <v>9</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>22</v>
       </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" t="n">
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="32" t="n">
+    <row r="27" spans="1:6">
+      <c r="A27" s="34" t="n">
         <v>43560.41666666666</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" t="n">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
         <v>9</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>23</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>11</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="32" t="n">
+    <row r="28" spans="1:6">
+      <c r="A28" s="34" t="n">
         <v>43560.41666666666</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" t="n">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
         <v>12</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>22</v>
       </c>
-      <c r="D28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" t="n">
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="32" t="n">
+    <row r="29" spans="1:6">
+      <c r="A29" s="34" t="n">
         <v>43560.41666666666</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" t="n">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
         <v>12</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>23</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>11</v>
       </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="32" t="n">
+    <row r="30" spans="1:6">
+      <c r="A30" s="34" t="n">
         <v>43560.41666666666</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" t="n">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
         <v>14</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>23</v>
       </c>
-      <c r="D30" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" t="n">
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="32" t="n">
+    <row r="31" spans="1:6">
+      <c r="A31" s="34" t="n">
         <v>43560.41666666666</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" t="n">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
         <v>14</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>23</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>11</v>
       </c>
-      <c r="E31" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="16" t="n">
-        <v>43559.20833333334</v>
-      </c>
-      <c r="B32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="16" t="n">
-        <v>43559.20833333334</v>
-      </c>
-      <c r="B33" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="16" t="n">
-        <v>43559.20833333334</v>
-      </c>
-      <c r="B34" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="16" t="n">
-        <v>43559.20833333334</v>
-      </c>
-      <c r="B35" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="16" t="n">
-        <v>43559.20833333334</v>
-      </c>
-      <c r="B36" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="16" t="n">
-        <v>43559.20833333334</v>
-      </c>
-      <c r="B37" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="16" t="n">
-        <v>43559.29166666666</v>
-      </c>
-      <c r="B38" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="16" t="n">
-        <v>43559.29166666666</v>
-      </c>
-      <c r="B39" t="s">
-        <v>21</v>
-      </c>
-      <c r="C39" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="16" t="n">
-        <v>43559.29166666666</v>
-      </c>
-      <c r="B40" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="16" t="n">
-        <v>43559.29166666666</v>
-      </c>
-      <c r="B41" t="s">
-        <v>23</v>
-      </c>
-      <c r="C41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="16" t="n">
-        <v>43559.29166666666</v>
-      </c>
-      <c r="B42" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" t="s">
-        <v>23</v>
-      </c>
-      <c r="D42" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="16" t="n">
-        <v>43559.29166666666</v>
-      </c>
-      <c r="B43" t="s">
-        <v>21</v>
-      </c>
-      <c r="C43" t="s">
-        <v>22</v>
-      </c>
-      <c r="D43" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="16" t="n">
-        <v>43559.29166666666</v>
-      </c>
-      <c r="B44" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="16" t="n">
-        <v>43559.29166666666</v>
-      </c>
-      <c r="B45" t="s">
-        <v>23</v>
-      </c>
-      <c r="C45" t="s">
-        <v>14</v>
-      </c>
-      <c r="D45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="16" t="n">
-        <v>43559.29166666666</v>
-      </c>
-      <c r="B46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46" t="s">
-        <v>21</v>
-      </c>
-      <c r="D46" t="s">
-        <v>10</v>
-      </c>
-      <c r="E46" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="16" t="n">
-        <v>43559.5</v>
-      </c>
-      <c r="B47" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="16" t="n">
-        <v>43559.5</v>
-      </c>
-      <c r="B48" t="s">
-        <v>21</v>
-      </c>
-      <c r="C48" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" t="s">
-        <v>10</v>
-      </c>
-      <c r="E48" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="16" t="n">
-        <v>43559.5</v>
-      </c>
-      <c r="B49" t="s">
-        <v>23</v>
-      </c>
-      <c r="C49" t="s">
-        <v>21</v>
-      </c>
-      <c r="D49" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="16" t="n">
-        <v>43560.04166666666</v>
-      </c>
-      <c r="B50" t="s">
-        <v>21</v>
-      </c>
-      <c r="C50" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="16" t="n">
-        <v>43560.04166666666</v>
-      </c>
-      <c r="B51" t="s">
-        <v>21</v>
-      </c>
-      <c r="C51" t="s">
-        <v>22</v>
-      </c>
-      <c r="D51" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="16" t="n">
-        <v>43560.04166666666</v>
-      </c>
-      <c r="B52" t="s">
-        <v>22</v>
-      </c>
-      <c r="C52" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" t="s">
-        <v>10</v>
-      </c>
-      <c r="E52" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="16" t="n">
-        <v>43560.04166666666</v>
-      </c>
-      <c r="B53" t="s">
-        <v>9</v>
-      </c>
-      <c r="C53" t="s">
-        <v>21</v>
-      </c>
-      <c r="D53" t="s">
-        <v>10</v>
-      </c>
-      <c r="E53" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="16" t="n">
-        <v>43560.04166666666</v>
-      </c>
-      <c r="B54" t="s">
-        <v>9</v>
-      </c>
-      <c r="C54" t="s">
-        <v>22</v>
-      </c>
-      <c r="D54" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="16" t="n">
-        <v>43560.04166666666</v>
-      </c>
-      <c r="B55" t="s">
-        <v>22</v>
-      </c>
-      <c r="C55" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="16" t="n">
-        <v>43560.04166666666</v>
-      </c>
-      <c r="B56" t="s">
-        <v>22</v>
-      </c>
-      <c r="C56" t="s">
-        <v>21</v>
-      </c>
-      <c r="D56" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="16" t="n">
-        <v>43560.04166666666</v>
-      </c>
-      <c r="B57" t="s">
-        <v>9</v>
-      </c>
-      <c r="C57" t="s">
-        <v>21</v>
-      </c>
-      <c r="D57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="16" t="n">
-        <v>43560.04166666666</v>
-      </c>
-      <c r="B58" t="s">
-        <v>21</v>
-      </c>
-      <c r="C58" t="s">
-        <v>22</v>
-      </c>
-      <c r="D58" t="s">
-        <v>10</v>
-      </c>
-      <c r="E58" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="16" t="n">
-        <v>43560.04166666666</v>
-      </c>
-      <c r="B59" t="s">
-        <v>22</v>
-      </c>
-      <c r="C59" t="s">
-        <v>12</v>
-      </c>
-      <c r="D59" t="s">
-        <v>10</v>
-      </c>
-      <c r="E59" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="16" t="n">
-        <v>43560.04166666666</v>
-      </c>
-      <c r="B60" t="s">
-        <v>23</v>
-      </c>
-      <c r="C60" t="s">
-        <v>21</v>
-      </c>
-      <c r="D60" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="16" t="n">
-        <v>43560.04166666666</v>
-      </c>
-      <c r="B61" t="s">
-        <v>12</v>
-      </c>
-      <c r="C61" t="s">
-        <v>22</v>
-      </c>
-      <c r="D61" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="16" t="n">
-        <v>43560.04166666666</v>
-      </c>
-      <c r="B62" t="s">
-        <v>21</v>
-      </c>
-      <c r="C62" t="s">
-        <v>22</v>
-      </c>
-      <c r="D62" t="s">
-        <v>10</v>
-      </c>
-      <c r="E62" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="16" t="n">
-        <v>43560.04166666666</v>
-      </c>
-      <c r="B63" t="s">
-        <v>22</v>
-      </c>
-      <c r="C63" t="s">
-        <v>12</v>
-      </c>
-      <c r="D63" t="s">
-        <v>11</v>
-      </c>
-      <c r="E63" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="16" t="n">
-        <v>43560.04166666666</v>
-      </c>
-      <c r="B64" t="s">
-        <v>23</v>
-      </c>
-      <c r="C64" t="s">
-        <v>21</v>
-      </c>
-      <c r="D64" t="s">
-        <v>10</v>
-      </c>
-      <c r="E64" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="16" t="n">
-        <v>43560.04166666666</v>
-      </c>
-      <c r="B65" t="s">
-        <v>23</v>
-      </c>
-      <c r="C65" t="s">
-        <v>22</v>
-      </c>
-      <c r="D65" t="s">
-        <v>10</v>
-      </c>
-      <c r="E65" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="16" t="n">
-        <v>43560.25</v>
-      </c>
-      <c r="B66" t="s">
-        <v>12</v>
-      </c>
-      <c r="C66" t="s">
-        <v>22</v>
-      </c>
-      <c r="D66" t="s">
-        <v>11</v>
-      </c>
-      <c r="E66" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="16" t="n">
-        <v>43560.25</v>
-      </c>
-      <c r="B67" t="s">
-        <v>21</v>
-      </c>
-      <c r="C67" t="s">
-        <v>9</v>
-      </c>
-      <c r="D67" t="s">
-        <v>10</v>
-      </c>
-      <c r="E67" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="16" t="n">
-        <v>43560.25</v>
-      </c>
-      <c r="B68" t="s">
-        <v>22</v>
-      </c>
-      <c r="C68" t="s">
-        <v>9</v>
-      </c>
-      <c r="D68" t="s">
-        <v>10</v>
-      </c>
-      <c r="E68" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="16" t="n">
-        <v>43560.25</v>
-      </c>
-      <c r="B69" t="s">
-        <v>23</v>
-      </c>
-      <c r="C69" t="s">
-        <v>21</v>
-      </c>
-      <c r="D69" t="s">
-        <v>10</v>
-      </c>
-      <c r="E69" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="16" t="n">
-        <v>43560.25</v>
-      </c>
-      <c r="B70" t="s">
-        <v>23</v>
-      </c>
-      <c r="C70" t="s">
-        <v>22</v>
-      </c>
-      <c r="D70" t="s">
-        <v>10</v>
-      </c>
-      <c r="E70" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="16" t="n">
-        <v>43560.25</v>
-      </c>
-      <c r="B71" t="s">
-        <v>9</v>
-      </c>
-      <c r="C71" t="s">
-        <v>21</v>
-      </c>
-      <c r="D71" t="s">
-        <v>10</v>
-      </c>
-      <c r="E71" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="16" t="n">
-        <v>43560.25</v>
-      </c>
-      <c r="B72" t="s">
-        <v>9</v>
-      </c>
-      <c r="C72" t="s">
-        <v>22</v>
-      </c>
-      <c r="D72" t="s">
-        <v>10</v>
-      </c>
-      <c r="E72" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" s="16" t="n">
-        <v>43560.25</v>
-      </c>
-      <c r="B73" t="s">
-        <v>21</v>
-      </c>
-      <c r="C73" t="s">
-        <v>9</v>
-      </c>
-      <c r="D73" t="s">
-        <v>11</v>
-      </c>
-      <c r="E73" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" s="16" t="n">
-        <v>43560.25</v>
-      </c>
-      <c r="B74" t="s">
-        <v>23</v>
-      </c>
-      <c r="C74" t="s">
-        <v>21</v>
-      </c>
-      <c r="D74" t="s">
-        <v>10</v>
-      </c>
-      <c r="E74" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
-      <c r="A75" s="16" t="n">
-        <v>43560.20833333334</v>
-      </c>
-      <c r="B75" t="s">
-        <v>9</v>
-      </c>
-      <c r="C75" t="s">
-        <v>21</v>
-      </c>
-      <c r="D75" t="s">
-        <v>11</v>
-      </c>
-      <c r="E75" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" s="16" t="n">
-        <v>43560.20833333334</v>
-      </c>
-      <c r="B76" t="s">
-        <v>21</v>
-      </c>
-      <c r="C76" t="s">
-        <v>22</v>
-      </c>
-      <c r="D76" t="s">
-        <v>10</v>
-      </c>
-      <c r="E76" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77" s="16" t="n">
-        <v>43560.20833333334</v>
-      </c>
-      <c r="B77" t="s">
-        <v>22</v>
-      </c>
-      <c r="C77" t="s">
-        <v>12</v>
-      </c>
-      <c r="D77" t="s">
-        <v>10</v>
-      </c>
-      <c r="E77" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="16" t="n">
-        <v>43560.20833333334</v>
-      </c>
-      <c r="B78" t="s">
-        <v>23</v>
-      </c>
-      <c r="C78" t="s">
-        <v>21</v>
-      </c>
-      <c r="D78" t="s">
-        <v>10</v>
-      </c>
-      <c r="E78" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="16" t="n">
-        <v>43560.20833333334</v>
-      </c>
-      <c r="B79" t="s">
-        <v>12</v>
-      </c>
-      <c r="C79" t="s">
-        <v>22</v>
-      </c>
-      <c r="D79" t="s">
-        <v>10</v>
-      </c>
-      <c r="E79" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
-      <c r="A80" s="16" t="n">
-        <v>43560.20833333334</v>
-      </c>
-      <c r="B80" t="s">
-        <v>21</v>
-      </c>
-      <c r="C80" t="s">
-        <v>22</v>
-      </c>
-      <c r="D80" t="s">
-        <v>10</v>
-      </c>
-      <c r="E80" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
-      <c r="A81" s="16" t="n">
-        <v>43560.20833333334</v>
-      </c>
-      <c r="B81" t="s">
-        <v>22</v>
-      </c>
-      <c r="C81" t="s">
-        <v>12</v>
-      </c>
-      <c r="D81" t="s">
-        <v>11</v>
-      </c>
-      <c r="E81" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
-      <c r="A82" s="16" t="n">
-        <v>43560.20833333334</v>
-      </c>
-      <c r="B82" t="s">
-        <v>23</v>
-      </c>
-      <c r="C82" t="s">
-        <v>21</v>
-      </c>
-      <c r="D82" t="s">
-        <v>10</v>
-      </c>
-      <c r="E82" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
-      <c r="A83" s="16" t="n">
-        <v>43560.20833333334</v>
-      </c>
-      <c r="B83" t="s">
-        <v>23</v>
-      </c>
-      <c r="C83" t="s">
-        <v>22</v>
-      </c>
-      <c r="D83" t="s">
-        <v>10</v>
-      </c>
-      <c r="E83" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
-      <c r="A84" s="16" t="n">
-        <v>43560.29166666666</v>
-      </c>
-      <c r="B84" t="s">
-        <v>12</v>
-      </c>
-      <c r="C84" t="s">
-        <v>22</v>
-      </c>
-      <c r="D84" t="s">
-        <v>11</v>
-      </c>
-      <c r="E84" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
-      <c r="A85" s="16" t="n">
-        <v>43560.29166666666</v>
-      </c>
-      <c r="B85" t="s">
-        <v>21</v>
-      </c>
-      <c r="C85" t="s">
-        <v>22</v>
-      </c>
-      <c r="D85" t="s">
-        <v>10</v>
-      </c>
-      <c r="E85" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
-      <c r="A86" s="16" t="n">
-        <v>43560.29166666666</v>
-      </c>
-      <c r="B86" t="s">
-        <v>21</v>
-      </c>
-      <c r="C86" t="s">
-        <v>23</v>
-      </c>
-      <c r="D86" t="s">
-        <v>10</v>
-      </c>
-      <c r="E86" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
-      <c r="A87" s="16" t="n">
-        <v>43560.29166666666</v>
-      </c>
-      <c r="B87" t="s">
-        <v>23</v>
-      </c>
-      <c r="C87" t="s">
-        <v>14</v>
-      </c>
-      <c r="D87" t="s">
-        <v>10</v>
-      </c>
-      <c r="E87" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
-      <c r="A88" s="16" t="n">
-        <v>43560.29166666666</v>
-      </c>
-      <c r="B88" t="s">
-        <v>14</v>
-      </c>
-      <c r="C88" t="s">
-        <v>23</v>
-      </c>
-      <c r="D88" t="s">
-        <v>10</v>
-      </c>
-      <c r="E88" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
-      <c r="A89" s="16" t="n">
-        <v>43560.29166666666</v>
-      </c>
-      <c r="B89" t="s">
-        <v>21</v>
-      </c>
-      <c r="C89" t="s">
-        <v>22</v>
-      </c>
-      <c r="D89" t="s">
-        <v>10</v>
-      </c>
-      <c r="E89" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5">
-      <c r="A90" s="16" t="n">
-        <v>43560.29166666666</v>
-      </c>
-      <c r="B90" t="s">
-        <v>23</v>
-      </c>
-      <c r="C90" t="s">
-        <v>14</v>
-      </c>
-      <c r="D90" t="s">
-        <v>11</v>
-      </c>
-      <c r="E90" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5">
-      <c r="A91" s="16" t="n">
-        <v>43560.29166666666</v>
-      </c>
-      <c r="B91" t="s">
-        <v>23</v>
-      </c>
-      <c r="C91" t="s">
-        <v>21</v>
-      </c>
-      <c r="D91" t="s">
-        <v>10</v>
-      </c>
-      <c r="E91" t="n">
+      <c r="F31" t="n">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Initial state now configured to pull from event rooms too
</commit_message>
<xml_diff>
--- a/DEAS_Equipment.xlsx
+++ b/DEAS_Equipment.xlsx
@@ -22,17 +22,13 @@
     <definedName name="StorageRooms">'Storage Rooms'!$A$2:$A$3</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Event Requirements'!$A$1:$H$1</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'Inventory by Room'!$A$1:$C$1</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Event Requirements'!$A$1:$H$1</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'Inventory by Room'!$A$1:$C$1</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Event Requirements'!$A$1:$H$1</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'Inventory by Room'!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <t>Event</t>
   </si>
@@ -82,46 +78,43 @@
     <t>E3</t>
   </si>
   <si>
-    <t>Chairs</t>
-  </si>
-  <si>
     <t>E4</t>
   </si>
   <si>
     <t>E5</t>
   </si>
   <si>
+    <t>Commodity</t>
+  </si>
+  <si>
+    <t>SR1</t>
+  </si>
+  <si>
+    <t>SR2</t>
+  </si>
+  <si>
+    <t>SR3</t>
+  </si>
+  <si>
+    <t>Event Room Room</t>
+  </si>
+  <si>
+    <t>Useful??</t>
+  </si>
+  <si>
+    <t>Units / Parcel</t>
+  </si>
+  <si>
+    <t>Volume/Parcel</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>ROUND</t>
+  </si>
+  <si>
     <t>Storage Room</t>
-  </si>
-  <si>
-    <t>Commodity</t>
-  </si>
-  <si>
-    <t>SR1</t>
-  </si>
-  <si>
-    <t>SR2</t>
-  </si>
-  <si>
-    <t>SR3</t>
-  </si>
-  <si>
-    <t>Event Room Room</t>
-  </si>
-  <si>
-    <t>Useful??</t>
-  </si>
-  <si>
-    <t>Units / Parcel</t>
-  </si>
-  <si>
-    <t>Volume/Parcel</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>ROUND</t>
   </si>
   <si>
     <t>Physical Capacity (sqft)</t>
@@ -173,10 +166,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt formatCode="[$-F400]h:mm:ss\ AM/PM" numFmtId="164"/>
-    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+    <numFmt formatCode="yyyy\-mm\-dd\ hh:mm:ss" numFmtId="165"/>
     <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="166"/>
+    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="167"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -400,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -448,12 +442,8 @@
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="13" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="13" fillId="3" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="13" fillId="2" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="2" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="3" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="13" fillId="3" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -767,7 +757,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="C6" pane="bottomLeft" sqref="C6"/>
+      <selection activeCell="G12" pane="bottomLeft" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -815,16 +805,16 @@
       <c r="B2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="29" t="n">
+      <c r="C2" s="22" t="n">
         <v>43559.04166666666</v>
       </c>
-      <c r="D2" s="29" t="n">
+      <c r="D2" s="22" t="n">
         <v>43559.08333333334</v>
       </c>
-      <c r="E2" s="29" t="n">
+      <c r="E2" s="22" t="n">
         <v>43559.125</v>
       </c>
-      <c r="F2" s="29" t="n">
+      <c r="F2" s="22" t="n">
         <v>43559.16666666666</v>
       </c>
       <c r="G2" s="21" t="s">
@@ -841,16 +831,16 @@
       <c r="B3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="30" t="n">
+      <c r="C3" s="17" t="n">
         <v>43559.04166666666</v>
       </c>
-      <c r="D3" s="30" t="n">
+      <c r="D3" s="17" t="n">
         <v>43559.08333333334</v>
       </c>
-      <c r="E3" s="30" t="n">
+      <c r="E3" s="17" t="n">
         <v>43559.125</v>
       </c>
-      <c r="F3" s="30" t="n">
+      <c r="F3" s="17" t="n">
         <v>43559.16666666666</v>
       </c>
       <c r="G3" s="16" t="s">
@@ -867,16 +857,16 @@
       <c r="B4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="30" t="n">
+      <c r="C4" s="17" t="n">
         <v>43559.04166666666</v>
       </c>
-      <c r="D4" s="30" t="n">
+      <c r="D4" s="17" t="n">
         <v>43559.08333333334</v>
       </c>
-      <c r="E4" s="30" t="n">
+      <c r="E4" s="17" t="n">
         <v>43559.125</v>
       </c>
-      <c r="F4" s="30" t="n">
+      <c r="F4" s="17" t="n">
         <v>43559.16666666666</v>
       </c>
       <c r="G4" s="16" t="s">
@@ -893,16 +883,16 @@
       <c r="B5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="30" t="n">
+      <c r="C5" s="17" t="n">
         <v>43559.04166666666</v>
       </c>
-      <c r="D5" s="30" t="n">
+      <c r="D5" s="17" t="n">
         <v>43559.08333333334</v>
       </c>
-      <c r="E5" s="30" t="n">
+      <c r="E5" s="17" t="n">
         <v>43559.125</v>
       </c>
-      <c r="F5" s="30" t="n">
+      <c r="F5" s="17" t="n">
         <v>43559.16666666666</v>
       </c>
       <c r="G5" s="16" t="s">
@@ -919,16 +909,16 @@
       <c r="B6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="30" t="n">
+      <c r="C6" s="17" t="n">
         <v>43559.25</v>
       </c>
-      <c r="D6" s="30" t="n">
+      <c r="D6" s="17" t="n">
         <v>43559.29166666666</v>
       </c>
-      <c r="E6" s="30" t="n">
+      <c r="E6" s="17" t="n">
         <v>43559.33333333334</v>
       </c>
-      <c r="F6" s="30" t="n">
+      <c r="F6" s="17" t="n">
         <v>43559.375</v>
       </c>
       <c r="G6" s="16" t="s">
@@ -945,16 +935,16 @@
       <c r="B7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="30" t="n">
+      <c r="C7" s="17" t="n">
         <v>43559.25</v>
       </c>
-      <c r="D7" s="30" t="n">
+      <c r="D7" s="17" t="n">
         <v>43559.29166666666</v>
       </c>
-      <c r="E7" s="30" t="n">
+      <c r="E7" s="17" t="n">
         <v>43559.33333333334</v>
       </c>
-      <c r="F7" s="30" t="n">
+      <c r="F7" s="17" t="n">
         <v>43559.375</v>
       </c>
       <c r="G7" s="16" t="s">
@@ -971,16 +961,16 @@
       <c r="B8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="31" t="n">
+      <c r="C8" s="19" t="n">
         <v>43559.20833333334</v>
       </c>
-      <c r="D8" s="31" t="n">
+      <c r="D8" s="19" t="n">
         <v>43559.25</v>
       </c>
-      <c r="E8" s="31" t="n">
+      <c r="E8" s="19" t="n">
         <v>43559.29166666666</v>
       </c>
-      <c r="F8" s="31" t="n">
+      <c r="F8" s="19" t="n">
         <v>43559.33333333334</v>
       </c>
       <c r="G8" s="18" t="s">
@@ -997,16 +987,16 @@
       <c r="B9" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="31" t="n">
+      <c r="C9" s="19" t="n">
         <v>43559.20833333334</v>
       </c>
-      <c r="D9" s="31" t="n">
+      <c r="D9" s="19" t="n">
         <v>43559.25</v>
       </c>
-      <c r="E9" s="31" t="n">
+      <c r="E9" s="19" t="n">
         <v>43559.29166666666</v>
       </c>
-      <c r="F9" s="31" t="n">
+      <c r="F9" s="19" t="n">
         <v>43559.33333333334</v>
       </c>
       <c r="G9" s="18" t="s">
@@ -1023,16 +1013,16 @@
       <c r="B10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="31" t="n">
+      <c r="C10" s="19" t="n">
         <v>43559.29166666666</v>
       </c>
-      <c r="D10" s="31" t="n">
+      <c r="D10" s="19" t="n">
         <v>43559.33333333334</v>
       </c>
-      <c r="E10" s="31" t="n">
+      <c r="E10" s="19" t="n">
         <v>43559.375</v>
       </c>
-      <c r="F10" s="31" t="n">
+      <c r="F10" s="19" t="n">
         <v>43559.41666666666</v>
       </c>
       <c r="G10" s="18" t="s">
@@ -1049,16 +1039,16 @@
       <c r="B11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="31" t="n">
+      <c r="C11" s="19" t="n">
         <v>43559.29166666666</v>
       </c>
-      <c r="D11" s="31" t="n">
+      <c r="D11" s="19" t="n">
         <v>43559.33333333334</v>
       </c>
-      <c r="E11" s="31" t="n">
+      <c r="E11" s="19" t="n">
         <v>43559.375</v>
       </c>
-      <c r="F11" s="31" t="n">
+      <c r="F11" s="19" t="n">
         <v>43559.41666666666</v>
       </c>
       <c r="G11" s="18" t="s">
@@ -1075,20 +1065,20 @@
       <c r="B12" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="30" t="n">
+      <c r="C12" s="17" t="n">
         <v>43559.5</v>
       </c>
-      <c r="D12" s="30" t="n">
+      <c r="D12" s="17" t="n">
         <v>43559.54166666666</v>
       </c>
-      <c r="E12" s="30" t="n">
+      <c r="E12" s="17" t="n">
         <v>43559.58333333334</v>
       </c>
-      <c r="F12" s="30" t="n">
+      <c r="F12" s="17" t="n">
         <v>43559.625</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H12" s="21" t="n">
         <v>30</v>
@@ -1096,21 +1086,21 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="32" t="n">
+      <c r="C13" s="28" t="n">
         <v>43560.04166666666</v>
       </c>
-      <c r="D13" s="32" t="n">
+      <c r="D13" s="28" t="n">
         <v>43560.08333333334</v>
       </c>
-      <c r="E13" s="32" t="n">
+      <c r="E13" s="28" t="n">
         <v>43560.125</v>
       </c>
-      <c r="F13" s="32" t="n">
+      <c r="F13" s="28" t="n">
         <v>43560.16666666666</v>
       </c>
       <c r="G13" s="27" t="s">
@@ -1122,21 +1112,21 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="32" t="n">
+      <c r="C14" s="28" t="n">
         <v>43560.04166666666</v>
       </c>
-      <c r="D14" s="32" t="n">
+      <c r="D14" s="28" t="n">
         <v>43560.08333333334</v>
       </c>
-      <c r="E14" s="32" t="n">
+      <c r="E14" s="28" t="n">
         <v>43560.125</v>
       </c>
-      <c r="F14" s="32" t="n">
+      <c r="F14" s="28" t="n">
         <v>43560.16666666666</v>
       </c>
       <c r="G14" s="18" t="s">
@@ -1148,21 +1138,21 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="32" t="n">
+      <c r="C15" s="28" t="n">
         <v>43560.04166666666</v>
       </c>
-      <c r="D15" s="32" t="n">
+      <c r="D15" s="28" t="n">
         <v>43560.08333333334</v>
       </c>
-      <c r="E15" s="32" t="n">
+      <c r="E15" s="28" t="n">
         <v>43560.125</v>
       </c>
-      <c r="F15" s="32" t="n">
+      <c r="F15" s="28" t="n">
         <v>43560.16666666666</v>
       </c>
       <c r="G15" s="18" t="s">
@@ -1174,21 +1164,21 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="32" t="n">
+      <c r="C16" s="28" t="n">
         <v>43560.04166666666</v>
       </c>
-      <c r="D16" s="32" t="n">
+      <c r="D16" s="28" t="n">
         <v>43560.08333333334</v>
       </c>
-      <c r="E16" s="32" t="n">
+      <c r="E16" s="28" t="n">
         <v>43560.125</v>
       </c>
-      <c r="F16" s="32" t="n">
+      <c r="F16" s="28" t="n">
         <v>43560.16666666666</v>
       </c>
       <c r="G16" s="18" t="s">
@@ -1200,21 +1190,21 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="31" t="n">
+      <c r="C17" s="19" t="n">
         <v>43560.25</v>
       </c>
-      <c r="D17" s="31" t="n">
+      <c r="D17" s="19" t="n">
         <v>43560.29166666666</v>
       </c>
-      <c r="E17" s="31" t="n">
+      <c r="E17" s="19" t="n">
         <v>43560.33333333334</v>
       </c>
-      <c r="F17" s="31" t="n">
+      <c r="F17" s="19" t="n">
         <v>43560.375</v>
       </c>
       <c r="G17" s="18" t="s">
@@ -1226,21 +1216,21 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="31" t="n">
+      <c r="C18" s="19" t="n">
         <v>43560.25</v>
       </c>
-      <c r="D18" s="31" t="n">
+      <c r="D18" s="19" t="n">
         <v>43560.29166666666</v>
       </c>
-      <c r="E18" s="31" t="n">
+      <c r="E18" s="19" t="n">
         <v>43560.33333333334</v>
       </c>
-      <c r="F18" s="31" t="n">
+      <c r="F18" s="19" t="n">
         <v>43560.375</v>
       </c>
       <c r="G18" s="18" t="s">
@@ -1252,21 +1242,21 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="30" t="n">
+      <c r="C19" s="17" t="n">
         <v>43560.20833333334</v>
       </c>
-      <c r="D19" s="30" t="n">
+      <c r="D19" s="17" t="n">
         <v>43560.25</v>
       </c>
-      <c r="E19" s="30" t="n">
+      <c r="E19" s="17" t="n">
         <v>43560.29166666666</v>
       </c>
-      <c r="F19" s="30" t="n">
+      <c r="F19" s="17" t="n">
         <v>43560.33333333334</v>
       </c>
       <c r="G19" s="16" t="s">
@@ -1278,21 +1268,21 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="30" t="n">
+      <c r="C20" s="17" t="n">
         <v>43560.20833333334</v>
       </c>
-      <c r="D20" s="30" t="n">
+      <c r="D20" s="17" t="n">
         <v>43560.25</v>
       </c>
-      <c r="E20" s="30" t="n">
+      <c r="E20" s="17" t="n">
         <v>43560.29166666666</v>
       </c>
-      <c r="F20" s="30" t="n">
+      <c r="F20" s="17" t="n">
         <v>43560.33333333334</v>
       </c>
       <c r="G20" s="16" t="s">
@@ -1304,21 +1294,21 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="30" t="n">
+      <c r="C21" s="17" t="n">
         <v>43560.29166666666</v>
       </c>
-      <c r="D21" s="30" t="n">
+      <c r="D21" s="17" t="n">
         <v>43560.33333333334</v>
       </c>
-      <c r="E21" s="30" t="n">
+      <c r="E21" s="17" t="n">
         <v>43560.375</v>
       </c>
-      <c r="F21" s="30" t="n">
+      <c r="F21" s="17" t="n">
         <v>43560.41666666666</v>
       </c>
       <c r="G21" s="16" t="s">
@@ -1330,21 +1320,21 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="30" t="n">
+      <c r="C22" s="17" t="n">
         <v>43560.29166666666</v>
       </c>
-      <c r="D22" s="30" t="n">
+      <c r="D22" s="17" t="n">
         <v>43560.33333333334</v>
       </c>
-      <c r="E22" s="30" t="n">
+      <c r="E22" s="17" t="n">
         <v>43560.375</v>
       </c>
-      <c r="F22" s="30" t="n">
+      <c r="F22" s="17" t="n">
         <v>43560.41666666666</v>
       </c>
       <c r="G22" s="16" t="s">
@@ -1949,11 +1939,11 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1:C1"/>
+      <selection activeCell="A7" pane="bottomLeft" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -1965,10 +1955,10 @@
   <sheetData>
     <row customHeight="1" ht="15" r="1" spans="1:3" thickBot="1">
       <c r="A1" s="23" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" s="25" t="s">
         <v>7</v>
@@ -1976,7 +1966,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -1987,7 +1977,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -1998,7 +1988,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -2009,7 +1999,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -2020,7 +2010,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -2031,13 +2021,79 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2066,10 +2122,10 @@
   <sheetData>
     <row customHeight="1" ht="15" r="1" spans="1:3" thickBot="1">
       <c r="A1" s="23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" s="25" t="s">
         <v>7</v>
@@ -2077,7 +2133,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2109,16 +2165,16 @@
   <sheetData>
     <row customHeight="1" ht="15" r="1" spans="1:4" thickBot="1">
       <c r="A1" s="23" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="25" t="s">
         <v>26</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>28</v>
       </c>
     </row>
     <row customHeight="1" ht="17" r="2" spans="1:4">
@@ -2151,7 +2207,7 @@
     </row>
     <row customHeight="1" ht="15" r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" t="n">
         <v>2</v>
@@ -2231,63 +2287,63 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>35</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="n"/>
       <c r="D2" t="n">
         <v>15</v>
       </c>
       <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
         <v>37</v>
-      </c>
-      <c r="H2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="n"/>
       <c r="D3" t="n">
         <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" t="n">
         <v>50</v>
@@ -2488,13 +2544,13 @@
         <v>14</v>
       </c>
       <c r="E1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2568,7 +2624,7 @@
     </row>
     <row customHeight="1" ht="15" r="5" spans="1:7">
       <c r="A5" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" t="n">
         <v>7</v>
@@ -2591,7 +2647,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="n">
         <v>9</v>
@@ -2614,7 +2670,7 @@
     </row>
     <row customHeight="1" ht="15" r="7" spans="1:7" thickBot="1">
       <c r="A7" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>10</v>
@@ -2646,43 +2702,43 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="34" t="n">
+      <c r="A2" s="30" t="n">
         <v>43559.04166666666</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -2695,34 +2751,34 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="34" t="n">
+      <c r="A3" s="30" t="n">
         <v>43559.04166666666</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="30" t="n">
+        <v>43559.04166666666</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="34" t="n">
-        <v>43559.04166666666</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -2731,18 +2787,18 @@
         <v>11</v>
       </c>
       <c r="F4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="34" t="n">
+      <c r="A5" s="30" t="n">
         <v>43559.04166666666</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -2755,14 +2811,14 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="34" t="n">
+      <c r="A6" s="30" t="n">
         <v>43559.04166666666</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -2775,54 +2831,54 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="34" t="n">
+      <c r="A7" s="30" t="n">
         <v>43559.04166666666</v>
       </c>
       <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="n">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="30" t="n">
+        <v>43559.04166666666</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="34" t="n">
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="30" t="n">
         <v>43559.04166666666</v>
       </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
         <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="34" t="n">
-        <v>43559.41666666666</v>
-      </c>
-      <c r="B9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
@@ -2831,121 +2887,121 @@
         <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="34" t="n">
-        <v>43559.41666666666</v>
+      <c r="A10" s="30" t="n">
+        <v>43559.04166666666</v>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F10" t="n">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="34" t="n">
-        <v>43559.41666666666</v>
+      <c r="A11" s="30" t="n">
+        <v>43559.16666666666</v>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="34" t="n">
-        <v>43559.41666666666</v>
+      <c r="A12" s="30" t="n">
+        <v>43559.16666666666</v>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="30" t="n">
+        <v>43559.16666666666</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="30" t="n">
+        <v>43559.16666666666</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" t="n">
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="34" t="n">
-        <v>43559.41666666666</v>
-      </c>
-      <c r="B13" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" s="30" t="n">
+        <v>43559.16666666666</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
         <v>12</v>
       </c>
-      <c r="D13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="34" t="n">
-        <v>43559.41666666666</v>
-      </c>
-      <c r="B14" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="34" t="n">
-        <v>43559.41666666666</v>
-      </c>
-      <c r="B15" t="n">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
@@ -2955,94 +3011,94 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="34" t="n">
-        <v>43559.41666666666</v>
+      <c r="A16" s="30" t="n">
+        <v>43559.16666666666</v>
       </c>
       <c r="B16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
         <v>21</v>
       </c>
-      <c r="D16" t="s">
-        <v>23</v>
-      </c>
       <c r="E16" t="s">
         <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="34" t="n">
-        <v>43559.5</v>
+      <c r="A17" s="30" t="n">
+        <v>43559.16666666666</v>
       </c>
       <c r="B17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
         <v>21</v>
       </c>
-      <c r="D17" t="s">
-        <v>22</v>
-      </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F17" t="n">
-        <v>55</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="34" t="n">
-        <v>43559.625</v>
+      <c r="A18" s="30" t="n">
+        <v>43559.16666666666</v>
       </c>
       <c r="B18" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
         <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="34" t="n">
-        <v>43560.04166666666</v>
+      <c r="A19" s="30" t="n">
+        <v>43559.16666666666</v>
       </c>
       <c r="B19" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F19" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="34" t="n">
-        <v>43560.04166666666</v>
+      <c r="A20" s="30" t="n">
+        <v>43559.20833333334</v>
       </c>
       <c r="B20" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
@@ -3051,38 +3107,38 @@
         <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="34" t="n">
-        <v>43560.04166666666</v>
+      <c r="A21" s="30" t="n">
+        <v>43559.20833333334</v>
       </c>
       <c r="B21" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="34" t="n">
-        <v>43560.04166666666</v>
+      <c r="A22" s="30" t="n">
+        <v>43559.20833333334</v>
       </c>
       <c r="B22" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
@@ -3091,187 +3147,1087 @@
         <v>11</v>
       </c>
       <c r="F22" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="34" t="n">
-        <v>43560.04166666666</v>
+      <c r="A23" s="30" t="n">
+        <v>43559.20833333334</v>
       </c>
       <c r="B23" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="34" t="n">
-        <v>43560.04166666666</v>
+      <c r="A24" s="30" t="n">
+        <v>43559.20833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="34" t="n">
-        <v>43560.41666666666</v>
+      <c r="A25" s="30" t="n">
+        <v>43559.20833333334</v>
       </c>
       <c r="B25" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" t="n">
         <v>6</v>
       </c>
-      <c r="C25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" t="s">
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="30" t="n">
+        <v>43559.20833333334</v>
+      </c>
+      <c r="B26" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
         <v>21</v>
       </c>
-      <c r="E25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="34" t="n">
-        <v>43560.41666666666</v>
-      </c>
-      <c r="B26" t="n">
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="30" t="n">
+        <v>43559.20833333334</v>
+      </c>
+      <c r="B27" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" t="n">
         <v>6</v>
       </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="34" t="n">
-        <v>43560.41666666666</v>
-      </c>
-      <c r="B27" t="n">
-        <v>6</v>
-      </c>
-      <c r="C27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" t="n">
-        <v>5</v>
-      </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="34" t="n">
-        <v>43560.41666666666</v>
+      <c r="A28" s="30" t="n">
+        <v>43559.25</v>
       </c>
       <c r="B28" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C28" t="s">
         <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="34" t="n">
-        <v>43560.41666666666</v>
+      <c r="A29" s="30" t="n">
+        <v>43559.25</v>
       </c>
       <c r="B29" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
         <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E29" t="s">
         <v>11</v>
       </c>
       <c r="F29" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="30" t="n">
+        <v>43559.25</v>
+      </c>
+      <c r="B30" t="n">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="30" t="n">
+        <v>43559.25</v>
+      </c>
+      <c r="B31" t="n">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="30" t="n">
+        <v>43559.25</v>
+      </c>
+      <c r="B32" t="n">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="34" t="n">
-        <v>43560.41666666666</v>
-      </c>
-      <c r="B30" t="n">
+    <row r="33" spans="1:6">
+      <c r="A33" s="30" t="n">
+        <v>43559.25</v>
+      </c>
+      <c r="B33" t="n">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="30" t="n">
+        <v>43559.25</v>
+      </c>
+      <c r="B34" t="n">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="30" t="n">
+        <v>43559.25</v>
+      </c>
+      <c r="B35" t="n">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="30" t="n">
+        <v>43559.25</v>
+      </c>
+      <c r="B36" t="n">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="30" t="n">
+        <v>43559.25</v>
+      </c>
+      <c r="B37" t="n">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" t="n">
         <v>6</v>
       </c>
-      <c r="C30" t="s">
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="30" t="n">
+        <v>43559.29166666666</v>
+      </c>
+      <c r="B38" t="n">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="30" t="n">
+        <v>43559.29166666666</v>
+      </c>
+      <c r="B39" t="n">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="30" t="n">
+        <v>43559.29166666666</v>
+      </c>
+      <c r="B40" t="n">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="30" t="n">
+        <v>43559.29166666666</v>
+      </c>
+      <c r="B41" t="n">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="30" t="n">
+        <v>43559.29166666666</v>
+      </c>
+      <c r="B42" t="n">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" t="s">
         <v>14</v>
       </c>
-      <c r="D30" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="34" t="n">
-        <v>43560.41666666666</v>
-      </c>
-      <c r="B31" t="n">
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="30" t="n">
+        <v>43559.29166666666</v>
+      </c>
+      <c r="B43" t="n">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="30" t="n">
+        <v>43559.29166666666</v>
+      </c>
+      <c r="B44" t="n">
+        <v>4</v>
+      </c>
+      <c r="C44" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="30" t="n">
+        <v>43559.29166666666</v>
+      </c>
+      <c r="B45" t="n">
+        <v>4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="30" t="n">
+        <v>43559.29166666666</v>
+      </c>
+      <c r="B46" t="n">
+        <v>4</v>
+      </c>
+      <c r="C46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="30" t="n">
+        <v>43559.29166666666</v>
+      </c>
+      <c r="B47" t="n">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="30" t="n">
+        <v>43559.29166666666</v>
+      </c>
+      <c r="B48" t="n">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="30" t="n">
+        <v>43559.33333333334</v>
+      </c>
+      <c r="B49" t="n">
+        <v>5</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="30" t="n">
+        <v>43559.33333333334</v>
+      </c>
+      <c r="B50" t="n">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="30" t="n">
+        <v>43559.33333333334</v>
+      </c>
+      <c r="B51" t="n">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="30" t="n">
+        <v>43559.33333333334</v>
+      </c>
+      <c r="B52" t="n">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="30" t="n">
+        <v>43559.33333333334</v>
+      </c>
+      <c r="B53" t="n">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" t="s">
+        <v>20</v>
+      </c>
+      <c r="E53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="30" t="n">
+        <v>43559.33333333334</v>
+      </c>
+      <c r="B54" t="n">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="30" t="n">
+        <v>43559.33333333334</v>
+      </c>
+      <c r="B55" t="n">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" t="s">
+        <v>14</v>
+      </c>
+      <c r="E55" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="30" t="n">
+        <v>43559.33333333334</v>
+      </c>
+      <c r="B56" t="n">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" t="s">
+        <v>20</v>
+      </c>
+      <c r="E56" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="30" t="n">
+        <v>43559.33333333334</v>
+      </c>
+      <c r="B57" t="n">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>20</v>
+      </c>
+      <c r="D57" t="s">
+        <v>20</v>
+      </c>
+      <c r="E57" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="30" t="n">
+        <v>43559.33333333334</v>
+      </c>
+      <c r="B58" t="n">
+        <v>5</v>
+      </c>
+      <c r="C58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D58" t="s">
+        <v>21</v>
+      </c>
+      <c r="E58" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="30" t="n">
+        <v>43559.33333333334</v>
+      </c>
+      <c r="B59" t="n">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s">
+        <v>21</v>
+      </c>
+      <c r="D59" t="s">
+        <v>21</v>
+      </c>
+      <c r="E59" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="30" t="n">
+        <v>43559.375</v>
+      </c>
+      <c r="B60" t="n">
         <v>6</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C60" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="30" t="n">
+        <v>43559.375</v>
+      </c>
+      <c r="B61" t="n">
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" t="s">
+        <v>20</v>
+      </c>
+      <c r="E61" t="s">
+        <v>11</v>
+      </c>
+      <c r="F61" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="30" t="n">
+        <v>43559.375</v>
+      </c>
+      <c r="B62" t="n">
+        <v>6</v>
+      </c>
+      <c r="C62" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="30" t="n">
+        <v>43559.375</v>
+      </c>
+      <c r="B63" t="n">
+        <v>6</v>
+      </c>
+      <c r="C63" t="s">
         <v>14</v>
       </c>
-      <c r="D31" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" t="n">
+      <c r="D63" t="s">
+        <v>14</v>
+      </c>
+      <c r="E63" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="30" t="n">
+        <v>43559.375</v>
+      </c>
+      <c r="B64" t="n">
+        <v>6</v>
+      </c>
+      <c r="C64" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" t="s">
+        <v>14</v>
+      </c>
+      <c r="E64" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="30" t="n">
+        <v>43559.375</v>
+      </c>
+      <c r="B65" t="n">
+        <v>6</v>
+      </c>
+      <c r="C65" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="30" t="n">
+        <v>43559.375</v>
+      </c>
+      <c r="B66" t="n">
+        <v>6</v>
+      </c>
+      <c r="C66" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" t="s">
+        <v>20</v>
+      </c>
+      <c r="E66" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="30" t="n">
+        <v>43559.375</v>
+      </c>
+      <c r="B67" t="n">
+        <v>6</v>
+      </c>
+      <c r="C67" t="s">
+        <v>20</v>
+      </c>
+      <c r="D67" t="s">
+        <v>20</v>
+      </c>
+      <c r="E67" t="s">
+        <v>11</v>
+      </c>
+      <c r="F67" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="30" t="n">
+        <v>43559.375</v>
+      </c>
+      <c r="B68" t="n">
+        <v>6</v>
+      </c>
+      <c r="C68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68" t="s">
+        <v>21</v>
+      </c>
+      <c r="E68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="30" t="n">
+        <v>43559.375</v>
+      </c>
+      <c r="B69" t="n">
+        <v>6</v>
+      </c>
+      <c r="C69" t="s">
+        <v>21</v>
+      </c>
+      <c r="D69" t="s">
+        <v>21</v>
+      </c>
+      <c r="E69" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="30" t="n">
+        <v>43559.375</v>
+      </c>
+      <c r="B70" t="n">
+        <v>6</v>
+      </c>
+      <c r="C70" t="s">
+        <v>21</v>
+      </c>
+      <c r="D70" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="30" t="n">
+        <v>43559.41666666666</v>
+      </c>
+      <c r="B71" t="n">
+        <v>7</v>
+      </c>
+      <c r="C71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" t="s">
+        <v>14</v>
+      </c>
+      <c r="E71" t="s">
+        <v>10</v>
+      </c>
+      <c r="F71" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="30" t="n">
+        <v>43559.41666666666</v>
+      </c>
+      <c r="B72" t="n">
+        <v>7</v>
+      </c>
+      <c r="C72" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" t="s">
+        <v>14</v>
+      </c>
+      <c r="E72" t="s">
+        <v>11</v>
+      </c>
+      <c r="F72" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="30" t="n">
+        <v>43559.41666666666</v>
+      </c>
+      <c r="B73" t="n">
+        <v>7</v>
+      </c>
+      <c r="C73" t="s">
+        <v>20</v>
+      </c>
+      <c r="D73" t="s">
+        <v>20</v>
+      </c>
+      <c r="E73" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="30" t="n">
+        <v>43559.41666666666</v>
+      </c>
+      <c r="B74" t="n">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s">
+        <v>20</v>
+      </c>
+      <c r="D74" t="s">
+        <v>20</v>
+      </c>
+      <c r="E74" t="s">
+        <v>11</v>
+      </c>
+      <c r="F74" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="30" t="n">
+        <v>43559.41666666666</v>
+      </c>
+      <c r="B75" t="n">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s">
+        <v>21</v>
+      </c>
+      <c r="D75" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" t="s">
+        <v>10</v>
+      </c>
+      <c r="F75" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="30" t="n">
+        <v>43559.41666666666</v>
+      </c>
+      <c r="B76" t="n">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s">
+        <v>21</v>
+      </c>
+      <c r="D76" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" t="s">
+        <v>11</v>
+      </c>
+      <c r="F76" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned a wkbk for new reqs, DEAS.xlsx
</commit_message>
<xml_diff>
--- a/DEAS_Equipment.xlsx
+++ b/DEAS_Equipment.xlsx
@@ -20,6 +20,10 @@
     <definedName name="Commodities">Commodities!$A$2:$A$3</definedName>
     <definedName name="Rooms">'Cost Data'!#REF!</definedName>
     <definedName name="StorageRooms">'Storage Rooms'!$A$2:$A$3</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Event Requirements'!$A$1:$H$1</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'Inventory by Room'!$A$1:$C$1</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Event Requirements'!$A$1:$H$1</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'Inventory by Room'!$A$1:$C$1</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Event Requirements'!$A$1:$H$1</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'Inventory by Room'!$A$1:$C$1</definedName>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Event Requirements'!$A$1:$H$1</definedName>
@@ -2711,7 +2715,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Changed invetory by room to just inventory
</commit_message>
<xml_diff>
--- a/DEAS_Equipment.xlsx
+++ b/DEAS_Equipment.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronnie\Desktop\DEAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F0263A-04DA-43F2-A8B2-265FE41E7452}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0950BF-4BB2-40BC-A83D-4AB96D5C10E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Event Requirements (2)" sheetId="1" r:id="rId1"/>
     <sheet name="Event Requirements" sheetId="2" r:id="rId2"/>
-    <sheet name="Inventory by Room" sheetId="3" r:id="rId3"/>
+    <sheet name="Inventory" sheetId="3" r:id="rId3"/>
     <sheet name="Deployed Units" sheetId="4" r:id="rId4"/>
     <sheet name="Commodities" sheetId="5" r:id="rId5"/>
     <sheet name="Storage Rooms" sheetId="6" r:id="rId6"/>
@@ -25,7 +25,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Event Requirements'!$A$1:$H$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Event Requirements (2)'!$A$1:$H$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Inventory by Room'!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Inventory!$A$1:$C$1</definedName>
     <definedName name="Commodities">Commodities!$A$2:$A$3</definedName>
     <definedName name="Rooms" localSheetId="0">'Cost Data'!#REF!</definedName>
     <definedName name="Rooms">'Cost Data'!#REF!</definedName>
@@ -775,7 +775,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12:H12"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1953,11 +1953,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H129"/>
+  <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8:H8"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2181,144 +2181,128 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="18"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
       <c r="G10" s="18"/>
       <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="18"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="27"/>
       <c r="B14" s="18"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
       <c r="G14" s="18"/>
       <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="27"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="27"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="27"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="27"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C33" s="2"/>
@@ -2877,30 +2861,6 @@
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>
-    </row>
-    <row r="126" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C126" s="2"/>
-      <c r="D126" s="2"/>
-      <c r="E126" s="2"/>
-      <c r="F126" s="2"/>
-    </row>
-    <row r="127" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C127" s="2"/>
-      <c r="D127" s="2"/>
-      <c r="E127" s="2"/>
-      <c r="F127" s="2"/>
-    </row>
-    <row r="128" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C128" s="2"/>
-      <c r="D128" s="2"/>
-      <c r="E128" s="2"/>
-      <c r="F128" s="2"/>
-    </row>
-    <row r="129" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C129" s="2"/>
-      <c r="D129" s="2"/>
-      <c r="E129" s="2"/>
-      <c r="F129" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
@@ -2913,7 +2873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>

</xml_diff>